<commit_message>
wat gerommel met populaties
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="17304" windowHeight="8112" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="17304" windowHeight="8112" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Bericht" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="282">
   <si>
     <t>ARAR Artikel 37a + 37b</t>
   </si>
@@ -689,456 +689,6 @@
     <t>wachtwoord</t>
   </si>
   <si>
-    <t>Zorina Abreu</t>
-  </si>
-  <si>
-    <t>Zhen Abu-Zahra</t>
-  </si>
-  <si>
-    <t>Zhanetta Adeyeye</t>
-  </si>
-  <si>
-    <t>Yunzhe Afonso</t>
-  </si>
-  <si>
-    <t>Youngjin Ahn</t>
-  </si>
-  <si>
-    <t>Yu Ahn</t>
-  </si>
-  <si>
-    <t>Yoon Akin-Aderibigbe</t>
-  </si>
-  <si>
-    <t>Yookyung Alexander</t>
-  </si>
-  <si>
-    <t>Yi-Shiuan Alsamdan</t>
-  </si>
-  <si>
-    <t>Yingda Alter</t>
-  </si>
-  <si>
-    <t>Ying Altmann</t>
-  </si>
-  <si>
-    <t>Yi-Feng Alvarez</t>
-  </si>
-  <si>
-    <t>Yi Aramendia</t>
-  </si>
-  <si>
-    <t>Yaya Ashkenazi</t>
-  </si>
-  <si>
-    <t>Yat-Lun Atri</t>
-  </si>
-  <si>
-    <t>Yasuhiro Au</t>
-  </si>
-  <si>
-    <t>Yanwen Aurori</t>
-  </si>
-  <si>
-    <t>Yan Austin</t>
-  </si>
-  <si>
-    <t>Ya-Han Bagdat</t>
-  </si>
-  <si>
-    <t>Yael Bala</t>
-  </si>
-  <si>
-    <t>Wushen Banovac</t>
-  </si>
-  <si>
-    <t>Won Barakat</t>
-  </si>
-  <si>
-    <t>Won Barnes</t>
-  </si>
-  <si>
-    <t>William Barrett</t>
-  </si>
-  <si>
-    <t>Willem Baxter</t>
-  </si>
-  <si>
-    <t>William Baxter</t>
-  </si>
-  <si>
-    <t>Wei Beatty</t>
-  </si>
-  <si>
-    <t>Wayne Bechrakis</t>
-  </si>
-  <si>
-    <t>Vivek Beistegui</t>
-  </si>
-  <si>
-    <t>Viacheslav Benchimol</t>
-  </si>
-  <si>
-    <t>Valle Berkman</t>
-  </si>
-  <si>
-    <t>Uros Birkhofer</t>
-  </si>
-  <si>
-    <t>Trent Blakely</t>
-  </si>
-  <si>
-    <t>Tobias Blattman</t>
-  </si>
-  <si>
-    <t>Timothy Bolton</t>
-  </si>
-  <si>
-    <t>Tiffanie Bosson</t>
-  </si>
-  <si>
-    <t>Thomas Brandt</t>
-  </si>
-  <si>
-    <t>Thomas Braun</t>
-  </si>
-  <si>
-    <t>Theodore Brodsky</t>
-  </si>
-  <si>
-    <t>Thavin Bromberg</t>
-  </si>
-  <si>
-    <t>Ted Brown</t>
-  </si>
-  <si>
-    <t>Thanadtha Brown</t>
-  </si>
-  <si>
-    <t>Taylor Buckley</t>
-  </si>
-  <si>
-    <t>Taryn Canal</t>
-  </si>
-  <si>
-    <t>Tara Cantrock</t>
-  </si>
-  <si>
-    <t>Tanzeer Cao</t>
-  </si>
-  <si>
-    <t>Tae Carrillo</t>
-  </si>
-  <si>
-    <t>Tadamitsu Carrow</t>
-  </si>
-  <si>
-    <t>Sung Casasayas</t>
-  </si>
-  <si>
-    <t>Suanne Cautero</t>
-  </si>
-  <si>
-    <t>Stuti Cha</t>
-  </si>
-  <si>
-    <t>Stephen Chan</t>
-  </si>
-  <si>
-    <t>Steven Chan</t>
-  </si>
-  <si>
-    <t>Sompop Chang</t>
-  </si>
-  <si>
-    <t>Spencer Chang</t>
-  </si>
-  <si>
-    <t>Stephanie Chang</t>
-  </si>
-  <si>
-    <t>Simond Chat</t>
-  </si>
-  <si>
-    <t>Simon Chau</t>
-  </si>
-  <si>
-    <t>Shiv Chayet</t>
-  </si>
-  <si>
-    <t>Shannon Cheesebro</t>
-  </si>
-  <si>
-    <t>Scott Chen</t>
-  </si>
-  <si>
-    <t>Se Chen</t>
-  </si>
-  <si>
-    <t>Sean Chen</t>
-  </si>
-  <si>
-    <t>Seth Chen</t>
-  </si>
-  <si>
-    <t>Sevag Chen</t>
-  </si>
-  <si>
-    <t>Scott Cheng</t>
-  </si>
-  <si>
-    <t>Satiya Cheung</t>
-  </si>
-  <si>
-    <t>Sarah Chin</t>
-  </si>
-  <si>
-    <t>Sara Chomitz</t>
-  </si>
-  <si>
-    <t>Samuel Chou</t>
-  </si>
-  <si>
-    <t>Sang Chou</t>
-  </si>
-  <si>
-    <t>Sangjo Chou</t>
-  </si>
-  <si>
-    <t>Samantha Chu</t>
-  </si>
-  <si>
-    <t>Samaneh Chua</t>
-  </si>
-  <si>
-    <t>Salas Chung</t>
-  </si>
-  <si>
-    <t>Saeed Cilento</t>
-  </si>
-  <si>
-    <t>Ryan Clark</t>
-  </si>
-  <si>
-    <t>Sachie Clark</t>
-  </si>
-  <si>
-    <t>Ryan Cloke</t>
-  </si>
-  <si>
-    <t>Rui Cockle</t>
-  </si>
-  <si>
-    <t>Roger Cooney</t>
-  </si>
-  <si>
-    <t>Roger Coyle</t>
-  </si>
-  <si>
-    <t>Rodriguez Crabtree</t>
-  </si>
-  <si>
-    <t>Robert Crunelle</t>
-  </si>
-  <si>
-    <t>Robert Cruse</t>
-  </si>
-  <si>
-    <t>Robert Cusnir</t>
-  </si>
-  <si>
-    <t>Robert Dahmubed</t>
-  </si>
-  <si>
-    <t>Robert Darby</t>
-  </si>
-  <si>
-    <t>Robert Davidowitz</t>
-  </si>
-  <si>
-    <t>Rikin Davis</t>
-  </si>
-  <si>
-    <t>Richard Dean</t>
-  </si>
-  <si>
-    <t>Richard Del</t>
-  </si>
-  <si>
-    <t>Remy Deomampo</t>
-  </si>
-  <si>
-    <t>Rahul Dickstein</t>
-  </si>
-  <si>
-    <t>Radu Donahue</t>
-  </si>
-  <si>
-    <t>Preston Doorey</t>
-  </si>
-  <si>
-    <t>Phill Doyle</t>
-  </si>
-  <si>
-    <t>Philip Druckman</t>
-  </si>
-  <si>
-    <t>Philip Duncan</t>
-  </si>
-  <si>
-    <t>Peter Elia</t>
-  </si>
-  <si>
-    <t>Peter Erickson</t>
-  </si>
-  <si>
-    <t>Peter Espinosa</t>
-  </si>
-  <si>
-    <t>Peter Ferrero</t>
-  </si>
-  <si>
-    <t>Perez Figueiredo</t>
-  </si>
-  <si>
-    <t>Patrick Fixler</t>
-  </si>
-  <si>
-    <t>Patrick Flegal</t>
-  </si>
-  <si>
-    <t>Patino Forsyth</t>
-  </si>
-  <si>
-    <t>Pallavi Fox</t>
-  </si>
-  <si>
-    <t>Owen Franzoni</t>
-  </si>
-  <si>
-    <t>Ophir Friedman</t>
-  </si>
-  <si>
-    <t>Obaid Friis</t>
-  </si>
-  <si>
-    <t>Noelle Fu</t>
-  </si>
-  <si>
-    <t>Noel Gambino</t>
-  </si>
-  <si>
-    <t>Nicole Gao</t>
-  </si>
-  <si>
-    <t>Nishant Gao</t>
-  </si>
-  <si>
-    <t>Nicole Garcia</t>
-  </si>
-  <si>
-    <t>Nicolas Gautam</t>
-  </si>
-  <si>
-    <t>Neto Gautier</t>
-  </si>
-  <si>
-    <t>Negrin Gee</t>
-  </si>
-  <si>
-    <t>Nawaz Georges</t>
-  </si>
-  <si>
-    <t>Nathan Gibb</t>
-  </si>
-  <si>
-    <t>Natalie Glenn</t>
-  </si>
-  <si>
-    <t>Nashat Goswamy</t>
-  </si>
-  <si>
-    <t>Nancy Goto</t>
-  </si>
-  <si>
-    <t>Muge Graves</t>
-  </si>
-  <si>
-    <t>Montero Greene</t>
-  </si>
-  <si>
-    <t>Mohtadi Greer</t>
-  </si>
-  <si>
-    <t>Mohammed Grisi</t>
-  </si>
-  <si>
-    <t>Miho Grobe</t>
-  </si>
-  <si>
-    <t>Michelle Grusq</t>
-  </si>
-  <si>
-    <t>Michael Guerra</t>
-  </si>
-  <si>
-    <t>Michael Guill</t>
-  </si>
-  <si>
-    <t>Michael Guinn</t>
-  </si>
-  <si>
-    <t>Micha Gupta</t>
-  </si>
-  <si>
-    <t>Michael Gupta</t>
-  </si>
-  <si>
-    <t>Maxwell Ha</t>
-  </si>
-  <si>
-    <t>Matthew Hagiwara</t>
-  </si>
-  <si>
-    <t>Matthew Hanan</t>
-  </si>
-  <si>
-    <t>Matthew Hawkins</t>
-  </si>
-  <si>
-    <t>Matthew Hersom</t>
-  </si>
-  <si>
-    <t>Matthew Hertzer</t>
-  </si>
-  <si>
-    <t>Matt Heshmatpour</t>
-  </si>
-  <si>
-    <t>Massimo Himmelfarb</t>
-  </si>
-  <si>
-    <t>Masayoshi Ho</t>
-  </si>
-  <si>
-    <t>Martinez Hofman</t>
-  </si>
-  <si>
-    <t>Martina Hofstee</t>
-  </si>
-  <si>
-    <t>Marshall Hoisington</t>
-  </si>
-  <si>
-    <t>Mark Holtz</t>
-  </si>
-  <si>
-    <t>Marissa Holzman</t>
-  </si>
-  <si>
-    <t>Maria Hong</t>
-  </si>
-  <si>
     <t>periodeResultaat</t>
   </si>
   <si>
@@ -1335,6 +885,9 @@
   </si>
   <si>
     <t>Roos Wijk</t>
+  </si>
+  <si>
+    <t>welkom</t>
   </si>
 </sst>
 </file>
@@ -2164,7 +1717,7 @@
         <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>366</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
         <v>139</v>
@@ -2179,7 +1732,7 @@
         <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>365</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2261,9 +1814,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3033,7 +2591,7 @@
         <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>367</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3064,7 +2622,7 @@
         <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>367</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3284,8 +2842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3347,16 +2905,16 @@
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>370</v>
+        <v>220</v>
       </c>
       <c r="E3" t="s">
-        <v>369</v>
+        <v>219</v>
       </c>
       <c r="F3" t="s">
         <v>144</v>
       </c>
       <c r="G3" t="s">
-        <v>368</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3365,7 +2923,7 @@
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>371</v>
+        <v>221</v>
       </c>
       <c r="E4" t="str">
         <f>E3</f>
@@ -3385,7 +2943,7 @@
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>372</v>
+        <v>222</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ref="E5:E56" si="0">E4</f>
@@ -3405,7 +2963,7 @@
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>373</v>
+        <v>223</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -3425,7 +2983,7 @@
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>374</v>
+        <v>224</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -3445,7 +3003,7 @@
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>375</v>
+        <v>225</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -3465,7 +3023,7 @@
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>226</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -3485,7 +3043,7 @@
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>377</v>
+        <v>227</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -3505,7 +3063,7 @@
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>378</v>
+        <v>228</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -3525,7 +3083,7 @@
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>379</v>
+        <v>229</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -3545,7 +3103,7 @@
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>380</v>
+        <v>230</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -3565,7 +3123,7 @@
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>381</v>
+        <v>231</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -3585,7 +3143,7 @@
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>382</v>
+        <v>232</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -3605,7 +3163,7 @@
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>383</v>
+        <v>233</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -3625,7 +3183,7 @@
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>384</v>
+        <v>234</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -3645,7 +3203,7 @@
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>385</v>
+        <v>235</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -3665,7 +3223,7 @@
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>386</v>
+        <v>236</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -3685,7 +3243,7 @@
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>387</v>
+        <v>237</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -3705,7 +3263,7 @@
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>388</v>
+        <v>238</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -3726,7 +3284,7 @@
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>389</v>
+        <v>239</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -3747,7 +3305,7 @@
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>390</v>
+        <v>240</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -3768,7 +3326,7 @@
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>391</v>
+        <v>241</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
@@ -3789,7 +3347,7 @@
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>392</v>
+        <v>242</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -3810,7 +3368,7 @@
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>393</v>
+        <v>243</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
@@ -3831,7 +3389,7 @@
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>394</v>
+        <v>244</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
@@ -3852,7 +3410,7 @@
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>395</v>
+        <v>245</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
@@ -3873,7 +3431,7 @@
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>396</v>
+        <v>246</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
@@ -3894,7 +3452,7 @@
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>397</v>
+        <v>247</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
@@ -3915,7 +3473,7 @@
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>398</v>
+        <v>248</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
@@ -3936,7 +3494,7 @@
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>399</v>
+        <v>249</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
@@ -3957,7 +3515,7 @@
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>400</v>
+        <v>250</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
@@ -3978,7 +3536,7 @@
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>401</v>
+        <v>251</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
@@ -3999,7 +3557,7 @@
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>402</v>
+        <v>252</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -4020,7 +3578,7 @@
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>403</v>
+        <v>253</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
@@ -4041,7 +3599,7 @@
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>404</v>
+        <v>254</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
@@ -4062,7 +3620,7 @@
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>405</v>
+        <v>255</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
@@ -4083,7 +3641,7 @@
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>406</v>
+        <v>256</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
@@ -4104,7 +3662,7 @@
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>407</v>
+        <v>257</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
@@ -4125,7 +3683,7 @@
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>408</v>
+        <v>258</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
@@ -4146,7 +3704,7 @@
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>409</v>
+        <v>259</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
@@ -4167,7 +3725,7 @@
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>410</v>
+        <v>260</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
@@ -4188,7 +3746,7 @@
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>411</v>
+        <v>261</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
@@ -4209,7 +3767,7 @@
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>412</v>
+        <v>262</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
@@ -4230,7 +3788,7 @@
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>413</v>
+        <v>263</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
@@ -4251,7 +3809,7 @@
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>414</v>
+        <v>264</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
@@ -4272,7 +3830,7 @@
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>415</v>
+        <v>265</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
@@ -4293,7 +3851,7 @@
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>416</v>
+        <v>266</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
@@ -4314,7 +3872,7 @@
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>417</v>
+        <v>267</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
@@ -4335,7 +3893,7 @@
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>418</v>
+        <v>268</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
@@ -4356,7 +3914,7 @@
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>419</v>
+        <v>269</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
@@ -4377,7 +3935,7 @@
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>420</v>
+        <v>270</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
@@ -4398,7 +3956,7 @@
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>421</v>
+        <v>271</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
@@ -4419,7 +3977,7 @@
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>422</v>
+        <v>272</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
@@ -4440,7 +3998,7 @@
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>423</v>
+        <v>273</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
@@ -4457,7 +4015,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>424</v>
+        <v>274</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="2"/>
@@ -4466,7 +4024,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>425</v>
+        <v>275</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="2"/>
@@ -4475,7 +4033,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>426</v>
+        <v>276</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="2"/>
@@ -4484,7 +4042,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>427</v>
+        <v>277</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="2"/>
@@ -4493,7 +4051,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>428</v>
+        <v>278</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="2"/>
@@ -4502,7 +4060,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>429</v>
+        <v>279</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="2"/>
@@ -4511,7 +4069,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>430</v>
+        <v>280</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="2"/>
@@ -4663,10 +4221,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I152"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4733,753 +4291,813 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>IF('[1]adhoc - Roosters '!A2,TEXT('[1]adhoc - Roosters '!A2,"#"),"")</f>
+        <v>7148691</v>
+      </c>
+      <c r="B3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
       <c r="I3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
+        <v>7151751</v>
+      </c>
+      <c r="B4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" t="s">
+        <v>281</v>
+      </c>
       <c r="I4" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
+        <v>20045763</v>
+      </c>
+      <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" t="s">
+        <v>281</v>
+      </c>
       <c r="I5" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
+        <v>20045773</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" t="s">
+        <v>281</v>
+      </c>
       <c r="I6" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
+        <v>20046068</v>
+      </c>
+      <c r="B7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" t="s">
+        <v>281</v>
+      </c>
       <c r="I7" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
+        <v>20046310</v>
+      </c>
+      <c r="B8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C8" t="s">
+        <v>281</v>
+      </c>
       <c r="I8" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
+        <v>20046336</v>
+      </c>
+      <c r="B9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C9" t="s">
+        <v>281</v>
+      </c>
       <c r="I9" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
+        <v>20046357</v>
+      </c>
+      <c r="B10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" t="s">
+        <v>281</v>
+      </c>
       <c r="I10" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
+        <v>20046480</v>
+      </c>
+      <c r="B11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" t="s">
+        <v>281</v>
+      </c>
       <c r="I11" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
+        <v>20046490</v>
+      </c>
+      <c r="B12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C12" t="s">
+        <v>281</v>
+      </c>
       <c r="I12" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
+        <v>20046544</v>
+      </c>
+      <c r="B13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" t="s">
+        <v>281</v>
+      </c>
       <c r="I13" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
+        <v>20046555</v>
+      </c>
+      <c r="B14" t="s">
+        <v>231</v>
+      </c>
+      <c r="C14" t="s">
+        <v>281</v>
+      </c>
       <c r="I14" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
+        <v>20046575</v>
+      </c>
+      <c r="B15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" t="s">
+        <v>281</v>
+      </c>
       <c r="I15" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
+        <v>20046636</v>
+      </c>
+      <c r="B16" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" t="s">
+        <v>281</v>
+      </c>
       <c r="I16" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
+        <v>20046659</v>
+      </c>
+      <c r="B17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" t="s">
+        <v>281</v>
+      </c>
       <c r="I17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
+        <v>20046686</v>
+      </c>
+      <c r="B18" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" t="s">
+        <v>281</v>
+      </c>
       <c r="I18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
+        <v>20046693</v>
+      </c>
+      <c r="B19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" t="s">
+        <v>281</v>
+      </c>
       <c r="I19" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
+        <v>20046747</v>
+      </c>
+      <c r="B20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C20" t="s">
+        <v>281</v>
+      </c>
       <c r="I20" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
+        <v>20046749</v>
+      </c>
+      <c r="B21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" t="s">
+        <v>281</v>
+      </c>
       <c r="I21" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
+        <v>20046812</v>
+      </c>
+      <c r="B22" t="s">
+        <v>239</v>
+      </c>
+      <c r="C22" t="s">
+        <v>281</v>
+      </c>
       <c r="I22" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
+        <v>20046859</v>
+      </c>
+      <c r="B23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C23" t="s">
+        <v>281</v>
+      </c>
       <c r="I23" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
+        <v>20046868</v>
+      </c>
+      <c r="B24" t="s">
+        <v>241</v>
+      </c>
+      <c r="C24" t="s">
+        <v>281</v>
+      </c>
       <c r="I24" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
+        <v>20046883</v>
+      </c>
+      <c r="B25" t="s">
+        <v>242</v>
+      </c>
+      <c r="C25" t="s">
+        <v>281</v>
+      </c>
       <c r="I25" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
+        <v>20046949</v>
+      </c>
+      <c r="B26" t="s">
+        <v>243</v>
+      </c>
+      <c r="C26" t="s">
+        <v>281</v>
+      </c>
       <c r="I26" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
+        <v>20046981</v>
+      </c>
+      <c r="B27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C27" t="s">
+        <v>281</v>
+      </c>
       <c r="I27" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
+        <v>20046987</v>
+      </c>
+      <c r="B28" t="s">
+        <v>245</v>
+      </c>
+      <c r="C28" t="s">
+        <v>281</v>
+      </c>
       <c r="I28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
+        <v>20047009</v>
+      </c>
+      <c r="B29" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29" t="s">
+        <v>281</v>
+      </c>
       <c r="I29" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
+        <v>20047081</v>
+      </c>
+      <c r="B30" t="s">
+        <v>247</v>
+      </c>
+      <c r="C30" t="s">
+        <v>281</v>
+      </c>
       <c r="I30" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
+        <v>20047085</v>
+      </c>
+      <c r="B31" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" t="s">
+        <v>281</v>
+      </c>
       <c r="I31" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
+        <v>20047108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>249</v>
+      </c>
+      <c r="C32" t="s">
+        <v>281</v>
+      </c>
       <c r="I32" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
+        <v>20047118</v>
+      </c>
+      <c r="B33" t="s">
+        <v>250</v>
+      </c>
+      <c r="C33" t="s">
+        <v>281</v>
+      </c>
       <c r="I33" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
+        <v>20047171</v>
+      </c>
+      <c r="B34" t="s">
+        <v>251</v>
+      </c>
+      <c r="C34" t="s">
+        <v>281</v>
+      </c>
       <c r="I34" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
+        <v>20047188</v>
+      </c>
+      <c r="B35" t="s">
+        <v>252</v>
+      </c>
+      <c r="C35" t="s">
+        <v>281</v>
+      </c>
       <c r="I35" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
+        <v>20047189</v>
+      </c>
+      <c r="B36" t="s">
+        <v>253</v>
+      </c>
+      <c r="C36" t="s">
+        <v>281</v>
+      </c>
       <c r="I36" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
+        <v>20047277</v>
+      </c>
+      <c r="B37" t="s">
+        <v>254</v>
+      </c>
+      <c r="C37" t="s">
+        <v>281</v>
+      </c>
       <c r="I37" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
+        <v>20047291</v>
+      </c>
+      <c r="B38" t="s">
+        <v>255</v>
+      </c>
+      <c r="C38" t="s">
+        <v>281</v>
+      </c>
       <c r="I38" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
+        <v>20047295</v>
+      </c>
+      <c r="B39" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" t="s">
+        <v>281</v>
+      </c>
       <c r="I39" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
+        <v>20047296</v>
+      </c>
+      <c r="B40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C40" t="s">
+        <v>281</v>
+      </c>
       <c r="I40" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
+        <v>20047310</v>
+      </c>
+      <c r="B41" t="s">
+        <v>258</v>
+      </c>
+      <c r="C41" t="s">
+        <v>281</v>
+      </c>
       <c r="I41" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
+        <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
+        <v>20047322</v>
+      </c>
+      <c r="B42" t="s">
+        <v>259</v>
+      </c>
+      <c r="C42" t="s">
+        <v>281</v>
+      </c>
       <c r="I42" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
+        <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
+        <v>20047330</v>
+      </c>
+      <c r="B43" t="s">
+        <v>260</v>
+      </c>
+      <c r="C43" t="s">
+        <v>281</v>
+      </c>
       <c r="I43" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
+        <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
+        <v>20047672</v>
+      </c>
+      <c r="B44" t="s">
+        <v>261</v>
+      </c>
+      <c r="C44" t="s">
+        <v>281</v>
+      </c>
       <c r="I44" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
+        <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
+        <v>20047692</v>
+      </c>
+      <c r="B45" t="s">
+        <v>262</v>
+      </c>
+      <c r="C45" t="s">
+        <v>281</v>
+      </c>
       <c r="I45" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
+        <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
+        <v>20047712</v>
+      </c>
+      <c r="B46" t="s">
+        <v>263</v>
+      </c>
+      <c r="C46" t="s">
+        <v>281</v>
+      </c>
       <c r="I46" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
+        <v>20047716</v>
+      </c>
+      <c r="B47" t="s">
+        <v>264</v>
+      </c>
+      <c r="C47" t="s">
+        <v>281</v>
+      </c>
       <c r="I47" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
+        <v>20047730</v>
+      </c>
+      <c r="B48" t="s">
+        <v>265</v>
+      </c>
+      <c r="C48" t="s">
+        <v>281</v>
+      </c>
       <c r="I48" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
+        <v>20047748</v>
+      </c>
+      <c r="B49" t="s">
+        <v>266</v>
+      </c>
+      <c r="C49" t="s">
+        <v>281</v>
+      </c>
       <c r="I49" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
+        <v>20047775</v>
+      </c>
+      <c r="B50" t="s">
+        <v>267</v>
+      </c>
+      <c r="C50" t="s">
+        <v>281</v>
+      </c>
       <c r="I50" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
+        <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
+        <v>20047776</v>
+      </c>
+      <c r="B51" t="s">
+        <v>268</v>
+      </c>
+      <c r="C51" t="s">
+        <v>281</v>
+      </c>
       <c r="I51" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
+        <v>20047805</v>
+      </c>
+      <c r="B52" t="s">
+        <v>269</v>
+      </c>
+      <c r="C52" t="s">
+        <v>281</v>
+      </c>
       <c r="I52" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
+        <v>20047807</v>
+      </c>
+      <c r="B53" t="s">
+        <v>270</v>
+      </c>
+      <c r="C53" t="s">
+        <v>281</v>
+      </c>
       <c r="I53" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
+        <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
+        <v>20047818</v>
+      </c>
+      <c r="B54" t="s">
+        <v>271</v>
+      </c>
+      <c r="C54" t="s">
+        <v>281</v>
+      </c>
       <c r="I54" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
+        <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
+        <v>20047832</v>
+      </c>
+      <c r="B55" t="s">
+        <v>272</v>
+      </c>
+      <c r="C55" t="s">
+        <v>281</v>
+      </c>
       <c r="I55" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
+        <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
+        <v>20047848</v>
+      </c>
+      <c r="B56" t="s">
+        <v>273</v>
+      </c>
+      <c r="C56" t="s">
+        <v>281</v>
+      </c>
       <c r="I56" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I57" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I58" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I59" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I60" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I61" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I62" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I63" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I64" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I65" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I66" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I67" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I68" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I69" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I70" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I71" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I72" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I73" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I74" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I75" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I76" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I77" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I78" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I79" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I80" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I81" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I82" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="83" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I83" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="84" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I84" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="85" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I85" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="86" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I86" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="87" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I87" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="88" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I88" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="89" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I89" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="90" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I90" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="91" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I91" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="92" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I92" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="93" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I93" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="94" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I94" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="95" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I95" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="96" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I96" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I97" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="98" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I98" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="99" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I99" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="100" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I100" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="101" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I101" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="102" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I102" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="103" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I103" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="104" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I104" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="105" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I105" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="106" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I106" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="107" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I107" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="108" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I108" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="109" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I109" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="110" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I110" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="111" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I111" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="112" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I112" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="113" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I113" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="114" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I114" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="115" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I115" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="116" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I116" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="117" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I117" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="118" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I118" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="119" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I119" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="120" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I120" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="121" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I121" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="122" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I122" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="123" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I123" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="124" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I124" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="125" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I125" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="126" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I126" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="127" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I127" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="128" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I128" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="129" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I129" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="130" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I130" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="131" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I131" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="132" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I132" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="133" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I133" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="134" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I134" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="135" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I135" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="136" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I136" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="137" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I137" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="138" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I138" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="139" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I139" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="140" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I140" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="141" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I141" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="142" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I142" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="143" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I143" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="144" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I144" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="145" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I145" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="146" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I146" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="147" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I147" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="148" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I148" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="149" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I149" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="150" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I150" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="151" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I151" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="152" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I152" t="s">
-        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rollen geregeld in adl script
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="17310" windowHeight="8115" firstSheet="6" activeTab="13"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Bericht" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="274">
   <si>
     <t>ARAR Artikel 37a + 37b</t>
   </si>
@@ -846,6 +846,24 @@
   </si>
   <si>
     <t>[Account]</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>FAB</t>
+  </si>
+  <si>
+    <t>P&amp;O</t>
+  </si>
+  <si>
+    <t>Medewerker</t>
+  </si>
+  <si>
+    <t>Leidinggevende</t>
   </si>
 </sst>
 </file>
@@ -885,7 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1190,29 +1208,29 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1250,7 +1268,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1322,7 +1340,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1502,7 +1520,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1555,7 +1573,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1586,7 +1604,7 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1668,15 +1686,15 @@
       <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1730,7 +1748,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1775,16 +1793,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1807,7 +1825,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1830,7 +1848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -1844,7 +1862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -1858,7 +1876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -1872,7 +1890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>181</v>
       </c>
@@ -1886,7 +1904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>182</v>
       </c>
@@ -1900,7 +1918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>183</v>
       </c>
@@ -1914,7 +1932,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>184</v>
       </c>
@@ -1928,7 +1946,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>185</v>
       </c>
@@ -1942,7 +1960,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>186</v>
       </c>
@@ -1956,7 +1974,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -1967,7 +1985,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -1978,7 +1996,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>180</v>
       </c>
@@ -1989,7 +2007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -2000,7 +2018,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>188</v>
       </c>
@@ -2011,7 +2029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -2022,7 +2040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>190</v>
       </c>
@@ -2033,7 +2051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -2044,7 +2062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -2055,7 +2073,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>159</v>
       </c>
@@ -2066,7 +2084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -2077,7 +2095,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>161</v>
       </c>
@@ -2088,7 +2106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -2099,7 +2117,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>163</v>
       </c>
@@ -2110,7 +2128,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>164</v>
       </c>
@@ -2121,7 +2139,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>165</v>
       </c>
@@ -2132,7 +2150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -2143,7 +2161,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>167</v>
       </c>
@@ -2154,7 +2172,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -2165,7 +2183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>170</v>
       </c>
@@ -2176,7 +2194,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>171</v>
       </c>
@@ -2187,7 +2205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -2198,7 +2216,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>173</v>
       </c>
@@ -2209,7 +2227,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -2220,7 +2238,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>175</v>
       </c>
@@ -2231,7 +2249,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>176</v>
       </c>
@@ -2253,7 +2271,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2282,7 +2300,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2311,7 +2329,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2340,7 +2358,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2369,7 +2387,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2398,7 +2416,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2427,7 +2445,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2456,7 +2474,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2485,7 +2503,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2514,7 +2532,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2545,7 +2563,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2576,7 +2594,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2607,10 +2625,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -2637,7 +2655,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2684,7 +2702,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2731,7 +2749,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2780,7 +2798,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2811,14 +2829,14 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -2832,7 +2850,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -2846,7 +2864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF('[1]adhoc - Roosters '!A2,TEXT('[1]adhoc - Roosters '!A2,"#"),"")</f>
         <v>7148691</v>
@@ -2861,7 +2879,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
         <v>7151751</v>
@@ -2877,7 +2895,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>20045763</v>
@@ -2893,7 +2911,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045773</v>
@@ -2909,7 +2927,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20046068</v>
@@ -2925,7 +2943,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046310</v>
@@ -2941,7 +2959,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046336</v>
@@ -2957,7 +2975,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046357</v>
@@ -2973,7 +2991,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046480</v>
@@ -2989,7 +3007,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046490</v>
@@ -3005,7 +3023,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046544</v>
@@ -3021,7 +3039,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046555</v>
@@ -3037,7 +3055,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046575</v>
@@ -3053,7 +3071,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046636</v>
@@ -3069,7 +3087,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046659</v>
@@ -3085,7 +3103,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046686</v>
@@ -3101,7 +3119,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046693</v>
@@ -3117,7 +3135,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046747</v>
@@ -3133,7 +3151,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046749</v>
@@ -3150,7 +3168,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046812</v>
@@ -3167,7 +3185,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046859</v>
@@ -3184,7 +3202,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046868</v>
@@ -3201,7 +3219,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046883</v>
@@ -3218,7 +3236,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046949</v>
@@ -3235,7 +3253,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046981</v>
@@ -3252,7 +3270,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046987</v>
@@ -3269,7 +3287,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20047009</v>
@@ -3286,7 +3304,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047081</v>
@@ -3303,7 +3321,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047085</v>
@@ -3320,7 +3338,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047108</v>
@@ -3337,7 +3355,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047118</v>
@@ -3354,7 +3372,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047171</v>
@@ -3371,7 +3389,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047188</v>
@@ -3388,7 +3406,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047189</v>
@@ -3405,7 +3423,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047277</v>
@@ -3422,7 +3440,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047291</v>
@@ -3439,7 +3457,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047295</v>
@@ -3456,7 +3474,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047296</v>
@@ -3473,7 +3491,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047310</v>
@@ -3490,7 +3508,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047322</v>
@@ -3507,7 +3525,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047330</v>
@@ -3524,7 +3542,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047672</v>
@@ -3541,7 +3559,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047692</v>
@@ -3558,7 +3576,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047712</v>
@@ -3575,7 +3593,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047716</v>
@@ -3592,7 +3610,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047730</v>
@@ -3609,7 +3627,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047748</v>
@@ -3626,7 +3644,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047775</v>
@@ -3643,7 +3661,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047776</v>
@@ -3660,7 +3678,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047805</v>
@@ -3677,7 +3695,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047807</v>
@@ -3694,7 +3712,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047818</v>
@@ -3711,7 +3729,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047832</v>
@@ -3728,7 +3746,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047848</v>
@@ -3745,7 +3763,7 @@
         <v>watIs_cat_Personeelsnummer</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>256</v>
       </c>
@@ -3754,7 +3772,7 @@
         <v>salarisschaal1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>257</v>
       </c>
@@ -3763,7 +3781,7 @@
         <v>salarisschaal2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>258</v>
       </c>
@@ -3772,7 +3790,7 @@
         <v>salarisschaal3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>259</v>
       </c>
@@ -3781,7 +3799,7 @@
         <v>salarisschaal4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>260</v>
       </c>
@@ -3790,7 +3808,7 @@
         <v>salarisschaal5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>261</v>
       </c>
@@ -3799,7 +3817,7 @@
         <v>salarisschaal6</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>262</v>
       </c>
@@ -3808,139 +3826,139 @@
         <v>salarisschaal7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C64" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal8</v>
       </c>
     </row>
-    <row r="65" spans="3:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal9</v>
       </c>
     </row>
-    <row r="66" spans="3:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal10</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" ht="15" x14ac:dyDescent="0.25">
       <c r="C67" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal11</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal12</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal13</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal14</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal15</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal16</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal17</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal18</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal1</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal2</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal3</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal4</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal5</v>
       </c>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal6</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal7</v>
       </c>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal8</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal9</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal10</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" t="str">
         <f t="shared" si="1"/>
         <v>salarisschaal11</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" t="str">
         <f t="shared" ref="C86" si="2">C68</f>
         <v>salarisschaal12</v>
@@ -3953,19 +3971,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>267</v>
       </c>
@@ -3978,8 +3998,11 @@
       <c r="D1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>266</v>
       </c>
@@ -3992,8 +4015,11 @@
       <c r="D2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF('[1]adhoc - Roosters '!A2,TEXT('[1]adhoc - Roosters '!A2,"#"),"")</f>
         <v>7148691</v>
@@ -4004,8 +4030,11 @@
       <c r="C3" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
         <v>7151751</v>
@@ -4016,8 +4045,11 @@
       <c r="C4" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>20045763</v>
@@ -4028,8 +4060,11 @@
       <c r="C5" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045773</v>
@@ -4040,8 +4075,11 @@
       <c r="C6" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20046068</v>
@@ -4052,8 +4090,11 @@
       <c r="C7" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046310</v>
@@ -4064,8 +4105,11 @@
       <c r="C8" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046336</v>
@@ -4076,8 +4120,11 @@
       <c r="C9" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046357</v>
@@ -4088,8 +4135,11 @@
       <c r="C10" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046480</v>
@@ -4100,8 +4150,11 @@
       <c r="C11" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046490</v>
@@ -4112,8 +4165,11 @@
       <c r="C12" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046544</v>
@@ -4124,8 +4180,11 @@
       <c r="C13" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046555</v>
@@ -4136,8 +4195,11 @@
       <c r="C14" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046575</v>
@@ -4148,8 +4210,11 @@
       <c r="C15" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046636</v>
@@ -4160,8 +4225,11 @@
       <c r="C16" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046659</v>
@@ -4172,8 +4240,11 @@
       <c r="C17" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046686</v>
@@ -4184,8 +4255,11 @@
       <c r="C18" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046693</v>
@@ -4196,8 +4270,11 @@
       <c r="C19" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046747</v>
@@ -4208,8 +4285,11 @@
       <c r="C20" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046749</v>
@@ -4220,8 +4300,11 @@
       <c r="C21" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046812</v>
@@ -4232,8 +4315,11 @@
       <c r="C22" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046859</v>
@@ -4244,8 +4330,11 @@
       <c r="C23" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046868</v>
@@ -4256,8 +4345,11 @@
       <c r="C24" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046883</v>
@@ -4268,8 +4360,11 @@
       <c r="C25" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046949</v>
@@ -4280,8 +4375,11 @@
       <c r="C26" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046981</v>
@@ -4292,8 +4390,11 @@
       <c r="C27" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046987</v>
@@ -4304,8 +4405,11 @@
       <c r="C28" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20047009</v>
@@ -4316,8 +4420,11 @@
       <c r="C29" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047081</v>
@@ -4328,8 +4435,11 @@
       <c r="C30" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047085</v>
@@ -4340,8 +4450,11 @@
       <c r="C31" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047108</v>
@@ -4352,8 +4465,11 @@
       <c r="C32" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047118</v>
@@ -4364,8 +4480,11 @@
       <c r="C33" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047171</v>
@@ -4376,8 +4495,11 @@
       <c r="C34" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047188</v>
@@ -4388,8 +4510,11 @@
       <c r="C35" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047189</v>
@@ -4400,8 +4525,11 @@
       <c r="C36" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047277</v>
@@ -4412,8 +4540,11 @@
       <c r="C37" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047291</v>
@@ -4424,8 +4555,11 @@
       <c r="C38" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047295</v>
@@ -4436,8 +4570,11 @@
       <c r="C39" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047296</v>
@@ -4448,8 +4585,11 @@
       <c r="C40" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047310</v>
@@ -4460,8 +4600,11 @@
       <c r="C41" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047322</v>
@@ -4472,8 +4615,11 @@
       <c r="C42" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047330</v>
@@ -4484,8 +4630,11 @@
       <c r="C43" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047672</v>
@@ -4496,8 +4645,11 @@
       <c r="C44" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047692</v>
@@ -4508,8 +4660,11 @@
       <c r="C45" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047712</v>
@@ -4520,8 +4675,11 @@
       <c r="C46" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047716</v>
@@ -4532,8 +4690,11 @@
       <c r="C47" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047730</v>
@@ -4544,8 +4705,11 @@
       <c r="C48" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047748</v>
@@ -4556,8 +4720,11 @@
       <c r="C49" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047775</v>
@@ -4568,8 +4735,11 @@
       <c r="C50" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E50" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047776</v>
@@ -4580,8 +4750,11 @@
       <c r="C51" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E51" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047805</v>
@@ -4592,8 +4765,11 @@
       <c r="C52" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E52" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047807</v>
@@ -4604,8 +4780,11 @@
       <c r="C53" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E53" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047818</v>
@@ -4616,8 +4795,11 @@
       <c r="C54" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="E54" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047832</v>
@@ -4628,8 +4810,11 @@
       <c r="C55" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047848</v>
@@ -4640,8 +4825,11 @@
       <c r="C56" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>264</v>
       </c>
@@ -4650,6 +4838,9 @@
       </c>
       <c r="C57" t="s">
         <v>263</v>
+      </c>
+      <c r="E57" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -4663,7 +4854,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
WIP. begrippen rechtgetrokken in FO en ADL
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Bericht" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="271">
   <si>
     <t>ARAR Artikel 37a + 37b</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>Salarisschalen</t>
-  </si>
-  <si>
-    <t>TEXT</t>
   </si>
   <si>
     <t>Tijdresultaat</t>
@@ -1518,25 +1515,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
       </c>
       <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" t="s">
         <v>194</v>
       </c>
-      <c r="D1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" t="s">
-        <v>195</v>
-      </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1571,15 +1568,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -1602,60 +1599,60 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" t="s">
         <v>96</v>
-      </c>
-      <c r="G1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" t="s">
-        <v>152</v>
-      </c>
-      <c r="M1" t="s">
-        <v>151</v>
-      </c>
-      <c r="N1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -1664,7 +1661,7 @@
         <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1693,27 +1690,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
         <v>125</v>
       </c>
-      <c r="D1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" t="s">
-        <v>126</v>
-      </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -1725,7 +1722,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -1746,33 +1743,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
         <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -1787,8 +1784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,39 +1795,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
         <v>192</v>
       </c>
-      <c r="D1" t="s">
-        <v>193</v>
-      </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -1839,18 +1833,18 @@
         <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>23</v>
@@ -1858,13 +1852,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
@@ -1872,13 +1866,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -1886,13 +1880,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
@@ -1900,13 +1894,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>23</v>
@@ -1914,13 +1908,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
@@ -1928,7 +1922,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -1942,7 +1936,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -1956,13 +1950,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
@@ -1970,32 +1964,32 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
@@ -2003,10 +1997,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
@@ -2014,10 +2008,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
@@ -2025,10 +2019,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
@@ -2036,10 +2030,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
@@ -2047,10 +2041,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
@@ -2058,10 +2052,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
@@ -2069,10 +2063,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F21" t="s">
         <v>39</v>
@@ -2080,10 +2074,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F22" t="s">
         <v>39</v>
@@ -2091,10 +2085,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F23" t="s">
         <v>39</v>
@@ -2102,10 +2096,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" t="s">
         <v>39</v>
@@ -2113,10 +2107,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F25" t="s">
         <v>39</v>
@@ -2124,10 +2118,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F26" t="s">
         <v>39</v>
@@ -2135,10 +2129,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F27" t="s">
         <v>39</v>
@@ -2146,10 +2140,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F28" t="s">
         <v>39</v>
@@ -2157,10 +2151,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F29" t="s">
         <v>39</v>
@@ -2168,10 +2162,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F30" t="s">
         <v>39</v>
@@ -2179,10 +2173,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F31" t="s">
         <v>39</v>
@@ -2190,10 +2184,10 @@
     </row>
     <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F32" t="s">
         <v>39</v>
@@ -2201,10 +2195,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
         <v>39</v>
@@ -2212,10 +2206,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F34" t="s">
         <v>39</v>
@@ -2223,10 +2217,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -2234,10 +2228,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F36" t="s">
         <v>39</v>
@@ -2245,10 +2239,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F37" t="s">
         <v>39</v>
@@ -2269,10 +2263,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2298,10 +2292,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2327,10 +2321,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2356,10 +2350,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2367,7 +2361,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2385,10 +2379,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2414,10 +2408,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2443,10 +2437,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2472,10 +2466,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2501,10 +2495,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2530,10 +2524,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2561,10 +2555,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2592,18 +2586,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2627,10 +2621,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2653,19 +2647,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,19 +2694,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2741,25 +2735,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" t="s">
-        <v>112</v>
-      </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2767,16 +2763,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2796,10 +2789,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2832,16 +2825,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2864,13 +2857,13 @@
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2879,10 +2872,10 @@
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" t="str">
         <f>D3</f>
@@ -2895,10 +2888,10 @@
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D56" si="0">D4</f>
@@ -2911,10 +2904,10 @@
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -2927,10 +2920,10 @@
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -2943,10 +2936,10 @@
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -2959,10 +2952,10 @@
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -2975,10 +2968,10 @@
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2991,10 +2984,10 @@
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -3007,10 +3000,10 @@
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -3023,10 +3016,10 @@
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -3039,10 +3032,10 @@
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -3055,10 +3048,10 @@
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -3071,10 +3064,10 @@
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -3087,10 +3080,10 @@
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -3103,10 +3096,10 @@
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -3119,10 +3112,10 @@
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -3135,10 +3128,10 @@
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -3151,7 +3144,7 @@
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C21" t="str">
         <f>C3</f>
@@ -3168,7 +3161,7 @@
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" ref="C22:C85" si="1">C4</f>
@@ -3185,7 +3178,7 @@
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
@@ -3202,7 +3195,7 @@
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
@@ -3219,7 +3212,7 @@
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
@@ -3236,7 +3229,7 @@
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
@@ -3253,7 +3246,7 @@
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
@@ -3270,7 +3263,7 @@
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
@@ -3287,7 +3280,7 @@
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
@@ -3304,7 +3297,7 @@
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
@@ -3321,7 +3314,7 @@
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
@@ -3338,7 +3331,7 @@
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
@@ -3355,7 +3348,7 @@
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
@@ -3372,7 +3365,7 @@
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
@@ -3389,7 +3382,7 @@
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
@@ -3406,7 +3399,7 @@
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
@@ -3423,7 +3416,7 @@
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
@@ -3440,7 +3433,7 @@
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
@@ -3457,7 +3450,7 @@
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
@@ -3474,7 +3467,7 @@
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
@@ -3491,7 +3484,7 @@
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
@@ -3508,7 +3501,7 @@
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
@@ -3525,7 +3518,7 @@
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
@@ -3542,7 +3535,7 @@
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
@@ -3559,7 +3552,7 @@
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
@@ -3576,7 +3569,7 @@
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
@@ -3593,7 +3586,7 @@
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
@@ -3610,7 +3603,7 @@
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
@@ -3627,7 +3620,7 @@
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
@@ -3644,7 +3637,7 @@
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
@@ -3661,7 +3654,7 @@
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
@@ -3678,7 +3671,7 @@
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
@@ -3695,7 +3688,7 @@
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -3712,7 +3705,7 @@
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -3729,7 +3722,7 @@
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -3746,7 +3739,7 @@
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -3759,7 +3752,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -3768,7 +3761,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -3777,7 +3770,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -3786,7 +3779,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -3795,7 +3788,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -3804,7 +3797,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -3813,7 +3806,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -3981,36 +3974,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
         <v>264</v>
-      </c>
-      <c r="B1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4019,13 +4012,13 @@
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4034,13 +4027,13 @@
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -4049,13 +4042,13 @@
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -4064,13 +4057,13 @@
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -4079,13 +4072,13 @@
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4094,13 +4087,13 @@
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -4109,13 +4102,13 @@
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -4124,13 +4117,13 @@
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -4139,13 +4132,13 @@
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -4154,13 +4147,13 @@
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -4169,13 +4162,13 @@
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -4184,13 +4177,13 @@
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -4199,13 +4192,13 @@
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -4214,13 +4207,13 @@
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -4229,13 +4222,13 @@
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -4244,13 +4237,13 @@
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -4259,13 +4252,13 @@
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -4274,13 +4267,13 @@
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -4289,13 +4282,13 @@
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -4304,13 +4297,13 @@
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -4319,13 +4312,13 @@
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -4334,13 +4327,13 @@
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C24" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -4349,13 +4342,13 @@
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -4364,13 +4357,13 @@
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -4379,13 +4372,13 @@
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -4394,13 +4387,13 @@
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -4409,13 +4402,13 @@
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -4424,13 +4417,13 @@
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -4439,13 +4432,13 @@
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -4454,13 +4447,13 @@
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -4469,13 +4462,13 @@
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -4484,13 +4477,13 @@
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -4499,13 +4492,13 @@
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E35" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -4514,13 +4507,13 @@
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -4529,13 +4522,13 @@
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E37" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -4544,13 +4537,13 @@
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -4559,13 +4552,13 @@
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -4574,13 +4567,13 @@
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E40" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -4589,13 +4582,13 @@
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C41" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E41" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -4604,13 +4597,13 @@
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -4619,13 +4612,13 @@
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E43" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -4634,13 +4627,13 @@
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C44" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E44" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -4649,13 +4642,13 @@
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E45" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -4664,13 +4657,13 @@
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -4679,13 +4672,13 @@
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E47" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -4694,13 +4687,13 @@
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E48" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -4709,13 +4702,13 @@
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -4724,13 +4717,13 @@
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E50" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -4739,13 +4732,13 @@
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C51" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E51" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -4754,13 +4747,13 @@
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -4769,13 +4762,13 @@
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E53" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -4784,13 +4777,13 @@
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C54" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E54" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -4799,13 +4792,13 @@
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C55" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E55" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -4814,13 +4807,13 @@
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E56" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4832,7 +4825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4840,13 +4833,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
         <v>148</v>
-      </c>
-      <c r="C1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4857,12 +4850,12 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work In Progress (WIP)
zet de berichten-interfaces van DTV.adl in één bestand: Berichten.adl
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -4,42 +4,40 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="9" r:id="rId1"/>
-    <sheet name="Dagresultaat" sheetId="2" r:id="rId2"/>
-    <sheet name="Dagverantwoording" sheetId="3" r:id="rId3"/>
-    <sheet name="MedewerkerRecht" sheetId="4" r:id="rId4"/>
-    <sheet name="Mutation" sheetId="6" r:id="rId5"/>
-    <sheet name="Personeelsnummer" sheetId="8" r:id="rId6"/>
-    <sheet name="SESSION" sheetId="10" r:id="rId7"/>
-    <sheet name="Tijdresultaat" sheetId="11" r:id="rId8"/>
-    <sheet name="Tijdvak" sheetId="12" r:id="rId9"/>
-    <sheet name="ToelageResultaat" sheetId="13" r:id="rId10"/>
-    <sheet name="Urentegoed" sheetId="14" r:id="rId11"/>
-    <sheet name="Variable" sheetId="15" r:id="rId12"/>
-    <sheet name="arbeidsmod" sheetId="17" r:id="rId13"/>
-    <sheet name="arbeidsmodaliteitIngangsdatum" sheetId="18" r:id="rId14"/>
-    <sheet name="binnenTijdvak" sheetId="19" r:id="rId15"/>
-    <sheet name="date" sheetId="20" r:id="rId16"/>
-    <sheet name="geldigOp" sheetId="21" r:id="rId17"/>
-    <sheet name="geqDatum" sheetId="22" r:id="rId18"/>
-    <sheet name="geqTijdstip" sheetId="23" r:id="rId19"/>
-    <sheet name="gtDatum" sheetId="24" r:id="rId20"/>
-    <sheet name="overlap1" sheetId="25" r:id="rId21"/>
-    <sheet name="overlap2" sheetId="26" r:id="rId22"/>
-    <sheet name="persoonsnr" sheetId="27" r:id="rId23"/>
+    <sheet name="Dagverantwoording" sheetId="3" r:id="rId2"/>
+    <sheet name="MedewerkerRecht" sheetId="4" r:id="rId3"/>
+    <sheet name="Mutation" sheetId="6" r:id="rId4"/>
+    <sheet name="Personeelsnummer" sheetId="8" r:id="rId5"/>
+    <sheet name="SESSION" sheetId="10" r:id="rId6"/>
+    <sheet name="Tijdvak" sheetId="12" r:id="rId7"/>
+    <sheet name="ToelageResultaat" sheetId="13" r:id="rId8"/>
+    <sheet name="Urentegoed" sheetId="14" r:id="rId9"/>
+    <sheet name="Variable" sheetId="15" r:id="rId10"/>
+    <sheet name="arbeidsmod" sheetId="17" r:id="rId11"/>
+    <sheet name="arbeidsmodaliteitIngangsdatum" sheetId="18" r:id="rId12"/>
+    <sheet name="binnenTijdvak" sheetId="19" r:id="rId13"/>
+    <sheet name="date" sheetId="20" r:id="rId14"/>
+    <sheet name="geldigOp" sheetId="21" r:id="rId15"/>
+    <sheet name="geqDatum" sheetId="22" r:id="rId16"/>
+    <sheet name="geqTijdstip" sheetId="23" r:id="rId17"/>
+    <sheet name="gtDatum" sheetId="24" r:id="rId18"/>
+    <sheet name="overlap1" sheetId="25" r:id="rId19"/>
+    <sheet name="overlap2" sheetId="26" r:id="rId20"/>
+    <sheet name="persoonsnr" sheetId="27" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId24"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="247">
   <si>
     <t>ARAR Artikel 37a + 37b</t>
   </si>
@@ -80,9 +78,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>Dagresultaat</t>
-  </si>
-  <si>
     <t>Dagsoort</t>
   </si>
   <si>
@@ -119,9 +114,6 @@
     <t>Overwerkverlof</t>
   </si>
   <si>
-    <t>Perioderesultaat</t>
-  </si>
-  <si>
     <t>Periodeverantwoording</t>
   </si>
   <si>
@@ -149,9 +141,6 @@
     <t>Salarisschalen</t>
   </si>
   <si>
-    <t>Tijdresultaat</t>
-  </si>
-  <si>
     <t>Tijdsduur</t>
   </si>
   <si>
@@ -203,9 +192,6 @@
     <t>[Arbeidsmodaliteit]</t>
   </si>
   <si>
-    <t>[Dagresultaat]</t>
-  </si>
-  <si>
     <t>[Dagverantwoording]</t>
   </si>
   <si>
@@ -236,9 +222,6 @@
     <t>[SrcTijdvak]</t>
   </si>
   <si>
-    <t>[Tijdresultaat]</t>
-  </si>
-  <si>
     <t>[Tijdvak]</t>
   </si>
   <si>
@@ -293,9 +276,6 @@
     <t>code</t>
   </si>
   <si>
-    <t>dag</t>
-  </si>
-  <si>
     <t>dag_Dienst</t>
   </si>
   <si>
@@ -345,9 +325,6 @@
   </si>
   <si>
     <t>mutNaam</t>
-  </si>
-  <si>
-    <t>periode</t>
   </si>
   <si>
     <t>periodenaam</t>
@@ -1465,36 +1442,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1503,13 +1480,13 @@
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1518,13 +1495,13 @@
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1533,13 +1510,13 @@
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" t="s">
         <v>242</v>
-      </c>
-      <c r="E5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1548,13 +1525,13 @@
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E6" t="s">
         <v>242</v>
-      </c>
-      <c r="E6" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1563,13 +1540,13 @@
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" t="s">
         <v>242</v>
-      </c>
-      <c r="E7" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1578,13 +1555,13 @@
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E8" t="s">
         <v>242</v>
-      </c>
-      <c r="E8" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1593,13 +1570,13 @@
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E9" t="s">
         <v>242</v>
-      </c>
-      <c r="E9" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1608,13 +1585,13 @@
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C10" t="s">
+        <v>235</v>
+      </c>
+      <c r="E10" t="s">
         <v>242</v>
-      </c>
-      <c r="E10" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1623,13 +1600,13 @@
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E11" t="s">
         <v>242</v>
-      </c>
-      <c r="E11" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1638,13 +1615,13 @@
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" t="s">
         <v>242</v>
-      </c>
-      <c r="E12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1653,13 +1630,13 @@
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
+        <v>235</v>
+      </c>
+      <c r="E13" t="s">
         <v>242</v>
-      </c>
-      <c r="E13" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1668,13 +1645,13 @@
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E14" t="s">
         <v>242</v>
-      </c>
-      <c r="E14" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1683,13 +1660,13 @@
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C15" t="s">
+        <v>235</v>
+      </c>
+      <c r="E15" t="s">
         <v>242</v>
-      </c>
-      <c r="E15" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1698,13 +1675,13 @@
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C16" t="s">
+        <v>235</v>
+      </c>
+      <c r="E16" t="s">
         <v>242</v>
-      </c>
-      <c r="E16" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1713,13 +1690,13 @@
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C17" t="s">
+        <v>235</v>
+      </c>
+      <c r="E17" t="s">
         <v>242</v>
-      </c>
-      <c r="E17" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1728,13 +1705,13 @@
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C18" t="s">
+        <v>235</v>
+      </c>
+      <c r="E18" t="s">
         <v>242</v>
-      </c>
-      <c r="E18" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1743,13 +1720,13 @@
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C19" t="s">
+        <v>235</v>
+      </c>
+      <c r="E19" t="s">
         <v>242</v>
-      </c>
-      <c r="E19" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1758,13 +1735,13 @@
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" t="s">
         <v>242</v>
-      </c>
-      <c r="E20" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1773,13 +1750,13 @@
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E21" t="s">
         <v>242</v>
-      </c>
-      <c r="E21" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1788,13 +1765,13 @@
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
+        <v>235</v>
+      </c>
+      <c r="E22" t="s">
         <v>242</v>
-      </c>
-      <c r="E22" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1803,13 +1780,13 @@
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C23" t="s">
+        <v>235</v>
+      </c>
+      <c r="E23" t="s">
         <v>242</v>
-      </c>
-      <c r="E23" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1818,13 +1795,13 @@
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E24" t="s">
         <v>242</v>
-      </c>
-      <c r="E24" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1833,13 +1810,13 @@
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C25" t="s">
+        <v>235</v>
+      </c>
+      <c r="E25" t="s">
         <v>242</v>
-      </c>
-      <c r="E25" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1848,13 +1825,13 @@
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C26" t="s">
+        <v>235</v>
+      </c>
+      <c r="E26" t="s">
         <v>242</v>
-      </c>
-      <c r="E26" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1863,13 +1840,13 @@
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C27" t="s">
+        <v>235</v>
+      </c>
+      <c r="E27" t="s">
         <v>242</v>
-      </c>
-      <c r="E27" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1878,13 +1855,13 @@
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C28" t="s">
+        <v>235</v>
+      </c>
+      <c r="E28" t="s">
         <v>242</v>
-      </c>
-      <c r="E28" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1893,13 +1870,13 @@
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C29" t="s">
+        <v>235</v>
+      </c>
+      <c r="E29" t="s">
         <v>242</v>
-      </c>
-      <c r="E29" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1908,13 +1885,13 @@
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C30" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E30" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1923,13 +1900,13 @@
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C31" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E31" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1938,13 +1915,13 @@
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E32" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1953,13 +1930,13 @@
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C33" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E33" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1968,13 +1945,13 @@
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C34" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E34" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1983,13 +1960,13 @@
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E35" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1998,13 +1975,13 @@
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E36" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2013,13 +1990,13 @@
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E37" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2028,13 +2005,13 @@
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E38" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2043,13 +2020,13 @@
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C39" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E39" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2058,13 +2035,13 @@
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C40" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E40" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2073,13 +2050,13 @@
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C41" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E41" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2088,13 +2065,13 @@
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C42" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E42" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2103,13 +2080,13 @@
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C43" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E43" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2118,13 +2095,13 @@
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C44" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E44" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2133,13 +2110,13 @@
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C45" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E45" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2148,13 +2125,13 @@
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C46" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E46" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2163,13 +2140,13 @@
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C47" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E47" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2178,13 +2155,13 @@
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C48" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E48" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2193,13 +2170,13 @@
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C49" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E49" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2208,13 +2185,13 @@
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C50" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E50" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2223,13 +2200,13 @@
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C51" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E51" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2238,13 +2215,13 @@
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C52" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E52" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2253,13 +2230,13 @@
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C53" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E53" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2268,13 +2245,13 @@
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C54" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E54" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2283,13 +2260,13 @@
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C55" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E55" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2298,13 +2275,13 @@
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="C56" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E56" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2313,112 +2290,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -2433,134 +2304,134 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -2569,65 +2440,65 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -2635,10 +2506,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
@@ -2646,10 +2517,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -2657,10 +2528,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -2668,10 +2539,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -2679,10 +2550,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -2690,200 +2561,258 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D20" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D25" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D33" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D36" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D37" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2901,7 +2830,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
@@ -2909,10 +2838,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2930,18 +2859,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2959,18 +2888,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2988,7 +2917,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>88</v>
@@ -2999,7 +2928,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3020,15 +2949,15 @@
         <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3046,18 +2975,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3069,24 +2998,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3095,6 +3026,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3106,47 +3080,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3155,68 +3100,6 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3232,15 +3115,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3258,36 +3141,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3296,53 +3179,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -3354,33 +3190,33 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" t="s">
-        <v>107</v>
-      </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3388,7 +3224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B63"/>
   <sheetViews>
@@ -3405,18 +3241,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3425,7 +3261,7 @@
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3434,7 +3270,7 @@
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3443,7 +3279,7 @@
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3452,7 +3288,7 @@
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3461,7 +3297,7 @@
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3470,7 +3306,7 @@
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3479,7 +3315,7 @@
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3488,7 +3324,7 @@
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3497,7 +3333,7 @@
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3506,7 +3342,7 @@
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3515,7 +3351,7 @@
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -3524,7 +3360,7 @@
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3533,7 +3369,7 @@
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3542,7 +3378,7 @@
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3551,7 +3387,7 @@
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3560,7 +3396,7 @@
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3569,7 +3405,7 @@
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3578,7 +3414,7 @@
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3587,7 +3423,7 @@
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3596,7 +3432,7 @@
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3605,7 +3441,7 @@
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3614,7 +3450,7 @@
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3623,7 +3459,7 @@
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3632,7 +3468,7 @@
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3641,7 +3477,7 @@
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3650,7 +3486,7 @@
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3659,7 +3495,7 @@
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3668,7 +3504,7 @@
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3677,7 +3513,7 @@
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3686,7 +3522,7 @@
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3695,7 +3531,7 @@
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3704,7 +3540,7 @@
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3713,7 +3549,7 @@
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3722,7 +3558,7 @@
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3731,7 +3567,7 @@
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3740,7 +3576,7 @@
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3749,7 +3585,7 @@
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3758,7 +3594,7 @@
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3767,7 +3603,7 @@
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3776,7 +3612,7 @@
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3785,7 +3621,7 @@
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3794,7 +3630,7 @@
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3803,7 +3639,7 @@
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3812,7 +3648,7 @@
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3821,7 +3657,7 @@
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3830,7 +3666,7 @@
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3839,7 +3675,7 @@
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3848,7 +3684,7 @@
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3857,7 +3693,7 @@
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3866,7 +3702,7 @@
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3875,7 +3711,7 @@
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3884,7 +3720,7 @@
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3893,7 +3729,7 @@
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3902,42 +3738,42 @@
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="B57" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="B58" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="B59" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="B60" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="B61" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="B62" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="B63" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3945,7 +3781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3957,29 +3793,111 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
         <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3989,26 +3907,54 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>245</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>246</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4018,79 +3964,46 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M1" t="s">
-        <v>135</v>
-      </c>
-      <c r="N1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hernoem ToelageResultaat naar Resultaat
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" activeTab="6"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="9" r:id="rId1"/>
@@ -162,9 +162,6 @@
     <t>Toelage t.g.v. ziekte</t>
   </si>
   <si>
-    <t>ToelageResultaat</t>
-  </si>
-  <si>
     <t>Urenpools</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>[Tijdvak]</t>
   </si>
   <si>
-    <t>[ToelageResultaat]</t>
-  </si>
-  <si>
     <t>[Urentegoed]</t>
   </si>
   <si>
@@ -778,6 +772,12 @@
   </si>
   <si>
     <t>OKresultaat</t>
+  </si>
+  <si>
+    <t>Resultaat</t>
+  </si>
+  <si>
+    <t>[Resultaat]</t>
   </si>
 </sst>
 </file>
@@ -1442,36 +1442,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1480,13 +1480,13 @@
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1495,13 +1495,13 @@
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1510,13 +1510,13 @@
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1525,13 +1525,13 @@
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1540,13 +1540,13 @@
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1555,13 +1555,13 @@
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1570,13 +1570,13 @@
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1585,13 +1585,13 @@
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1600,13 +1600,13 @@
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1615,13 +1615,13 @@
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1630,13 +1630,13 @@
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1645,13 +1645,13 @@
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1660,13 +1660,13 @@
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1675,13 +1675,13 @@
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1690,13 +1690,13 @@
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1705,13 +1705,13 @@
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1720,13 +1720,13 @@
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1735,13 +1735,13 @@
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1750,13 +1750,13 @@
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E21" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1765,13 +1765,13 @@
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1780,13 +1780,13 @@
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1795,13 +1795,13 @@
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1810,13 +1810,13 @@
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1825,13 +1825,13 @@
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1840,13 +1840,13 @@
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1855,13 +1855,13 @@
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E28" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1870,13 +1870,13 @@
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E29" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1885,13 +1885,13 @@
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E30" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1900,13 +1900,13 @@
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E31" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1915,13 +1915,13 @@
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C32" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1930,13 +1930,13 @@
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C33" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1945,13 +1945,13 @@
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C34" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1960,13 +1960,13 @@
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E35" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1975,13 +1975,13 @@
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C36" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E36" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1990,13 +1990,13 @@
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2005,13 +2005,13 @@
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E38" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2020,13 +2020,13 @@
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2035,13 +2035,13 @@
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E40" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2050,13 +2050,13 @@
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E41" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2065,13 +2065,13 @@
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C42" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E42" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2080,13 +2080,13 @@
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C43" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E43" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2095,13 +2095,13 @@
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C44" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E44" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2110,13 +2110,13 @@
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C45" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2125,13 +2125,13 @@
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C46" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E46" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2140,13 +2140,13 @@
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C47" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E47" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2155,13 +2155,13 @@
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C48" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E48" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2170,13 +2170,13 @@
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C49" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E49" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2185,13 +2185,13 @@
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2200,13 +2200,13 @@
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C51" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E51" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2215,13 +2215,13 @@
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C52" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E52" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2230,13 +2230,13 @@
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C53" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E53" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2245,13 +2245,13 @@
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C54" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E54" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2260,13 +2260,13 @@
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C55" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E55" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2275,13 +2275,13 @@
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C56" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E56" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2304,36 +2304,36 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -2342,18 +2342,18 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2375,7 +2375,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -2403,13 +2403,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -2417,13 +2417,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -2445,7 +2445,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -2473,32 +2473,32 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D12" t="s">
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -2506,10 +2506,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
@@ -2517,10 +2517,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -2528,10 +2528,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -2539,10 +2539,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
@@ -2550,10 +2550,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
@@ -2561,10 +2561,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F20" t="s">
         <v>33</v>
@@ -2572,10 +2572,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F21" t="s">
         <v>33</v>
@@ -2583,10 +2583,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
         <v>33</v>
@@ -2594,10 +2594,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
         <v>33</v>
@@ -2605,10 +2605,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F24" t="s">
         <v>33</v>
@@ -2616,10 +2616,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F25" t="s">
         <v>33</v>
@@ -2627,10 +2627,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F26" t="s">
         <v>33</v>
@@ -2638,10 +2638,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F27" t="s">
         <v>33</v>
@@ -2649,10 +2649,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F28" t="s">
         <v>33</v>
@@ -2660,10 +2660,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -2671,10 +2671,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F30" t="s">
         <v>33</v>
@@ -2682,10 +2682,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F31" t="s">
         <v>33</v>
@@ -2693,10 +2693,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F32" t="s">
         <v>33</v>
@@ -2704,10 +2704,10 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F33" t="s">
         <v>33</v>
@@ -2715,10 +2715,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F34" t="s">
         <v>33</v>
@@ -2726,10 +2726,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F35" t="s">
         <v>33</v>
@@ -2737,10 +2737,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F36" t="s">
         <v>33</v>
@@ -2748,10 +2748,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F37" t="s">
         <v>33</v>
@@ -2772,10 +2772,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2801,10 +2801,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2830,10 +2830,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2859,10 +2859,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2888,10 +2888,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2917,10 +2917,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2946,10 +2946,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2975,10 +2975,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3006,10 +3006,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3037,16 +3037,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3080,10 +3080,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3115,10 +3115,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3141,19 +3141,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3190,19 +3190,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3210,13 +3210,13 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3241,10 +3241,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3261,7 +3261,7 @@
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3270,7 +3270,7 @@
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3279,7 +3279,7 @@
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3288,7 +3288,7 @@
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3297,7 +3297,7 @@
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3306,7 +3306,7 @@
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3315,7 +3315,7 @@
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3324,7 +3324,7 @@
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3333,7 +3333,7 @@
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3342,7 +3342,7 @@
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3351,7 +3351,7 @@
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -3360,7 +3360,7 @@
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3369,7 +3369,7 @@
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3378,7 +3378,7 @@
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3387,7 +3387,7 @@
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3396,7 +3396,7 @@
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3405,7 +3405,7 @@
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3414,7 +3414,7 @@
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3423,7 +3423,7 @@
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3432,7 +3432,7 @@
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3441,7 +3441,7 @@
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3450,7 +3450,7 @@
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3459,7 +3459,7 @@
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3468,7 +3468,7 @@
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3477,7 +3477,7 @@
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3486,7 +3486,7 @@
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3495,7 +3495,7 @@
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3504,7 +3504,7 @@
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3513,7 +3513,7 @@
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3522,7 +3522,7 @@
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3531,7 +3531,7 @@
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3540,7 +3540,7 @@
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3549,7 +3549,7 @@
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3558,7 +3558,7 @@
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3567,7 +3567,7 @@
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3576,7 +3576,7 @@
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3585,7 +3585,7 @@
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3594,7 +3594,7 @@
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3603,7 +3603,7 @@
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3612,7 +3612,7 @@
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3621,7 +3621,7 @@
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3630,7 +3630,7 @@
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3639,7 +3639,7 @@
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3648,7 +3648,7 @@
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3657,7 +3657,7 @@
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -3666,7 +3666,7 @@
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3675,7 +3675,7 @@
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3684,7 +3684,7 @@
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3693,7 +3693,7 @@
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3702,7 +3702,7 @@
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3711,7 +3711,7 @@
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3720,7 +3720,7 @@
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3729,7 +3729,7 @@
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3738,42 +3738,42 @@
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="B57" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="B58" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="B59" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="B60" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="B61" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="B62" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="B63" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3793,13 +3793,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3810,12 +3810,12 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3827,7 +3827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -3835,7 +3835,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -3844,37 +3844,37 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3888,7 +3888,7 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
@@ -3909,9 +3909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -3925,27 +3923,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -3974,24 +3972,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
wijzig persoonsnr in account~
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="17310" windowHeight="8115" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
   <externalReferences>
     <externalReference r:id="rId22"/>
   </externalReferences>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -108,9 +108,6 @@
     <t>Mutation</t>
   </si>
   <si>
-    <t>Naam</t>
-  </si>
-  <si>
     <t>Overwerkverlof</t>
   </si>
   <si>
@@ -778,13 +775,16 @@
   </si>
   <si>
     <t>[Resultaat]</t>
+  </si>
+  <si>
+    <t>TEXT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -830,7 +830,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="adhoc - Roosters "/>
@@ -1142,7 +1142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -1216,6 +1216,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1250,6 +1251,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1425,863 +1427,863 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
         <v>235</v>
       </c>
-      <c r="B1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF('[1]adhoc - Roosters '!A2,TEXT('[1]adhoc - Roosters '!A2,"#"),"")</f>
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E10" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E12" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E13" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E14" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E15" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E16" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E17" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E18" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E19" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E20" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E23" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E24" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E25" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E26" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E29" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E30" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E31" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E32" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E33" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E34" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E36" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E37" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E38" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E39" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C40" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E40" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E41" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E42" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E43" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E44" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E45" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E46" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E47" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E48" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E49" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E50" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E51" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C52" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E52" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E53" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C54" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E54" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E55" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E56" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2290,148 +2292,148 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
         <v>167</v>
       </c>
-      <c r="D1" t="s">
-        <v>168</v>
-      </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -2443,318 +2445,318 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" t="s">
         <v>105</v>
       </c>
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" t="s">
-        <v>119</v>
-      </c>
-      <c r="F25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" t="s">
-        <v>120</v>
-      </c>
-      <c r="F26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>139</v>
-      </c>
-      <c r="D27" t="s">
-        <v>121</v>
-      </c>
-      <c r="F27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>140</v>
-      </c>
-      <c r="D28" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>141</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>106</v>
       </c>
-      <c r="F29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" t="s">
         <v>107</v>
       </c>
-      <c r="F30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
+      <c r="F31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>144</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>108</v>
       </c>
-      <c r="F31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>145</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>109</v>
       </c>
-      <c r="F32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>146</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>110</v>
       </c>
-      <c r="F33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>147</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>111</v>
       </c>
-      <c r="F34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
+      <c r="F35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>148</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>112</v>
       </c>
-      <c r="F35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
+      <c r="F36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>149</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>113</v>
       </c>
-      <c r="F36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>150</v>
-      </c>
-      <c r="D37" t="s">
-        <v>114</v>
-      </c>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2763,22 +2765,22 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2792,22 +2794,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2821,27 +2823,27 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2850,22 +2852,22 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2879,22 +2881,22 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2908,22 +2910,22 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2937,22 +2939,22 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2966,22 +2968,22 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2995,24 +2997,24 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3026,30 +3028,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3060,7 +3062,7 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3069,29 +3071,29 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3100,30 +3102,30 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3132,31 +3134,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3167,10 +3169,10 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3179,44 +3181,44 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3225,555 +3227,555 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF('[1]adhoc - Roosters '!A2,TEXT('[1]adhoc - Roosters '!A2,"#"),"")</f>
         <v>7148691</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
         <v>7151751</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>20045763</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045773</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20046068</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046310</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046336</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046357</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046480</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046490</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046544</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046555</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046575</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046636</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046659</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046686</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046693</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046747</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046749</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046812</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046859</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046868</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046883</v>
       </c>
       <c r="B25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046949</v>
       </c>
       <c r="B26" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046981</v>
       </c>
       <c r="B27" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046987</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20047009</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047081</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047085</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047108</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047118</v>
       </c>
       <c r="B33" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047171</v>
       </c>
       <c r="B34" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047188</v>
       </c>
       <c r="B35" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047189</v>
       </c>
       <c r="B36" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047277</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047291</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047295</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047296</v>
       </c>
       <c r="B40" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047310</v>
       </c>
       <c r="B41" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047322</v>
       </c>
       <c r="B42" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047330</v>
       </c>
       <c r="B43" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047672</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047692</v>
       </c>
       <c r="B45" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047712</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047716</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047730</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047748</v>
       </c>
       <c r="B49" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047775</v>
       </c>
       <c r="B50" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047776</v>
       </c>
       <c r="B51" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047805</v>
       </c>
       <c r="B52" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047807</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047818</v>
       </c>
       <c r="B54" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047832</v>
       </c>
       <c r="B55" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047848</v>
       </c>
       <c r="B56" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="B57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="B58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="B59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="B60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="B61" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="B62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="B63" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3782,40 +3784,40 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3824,71 +3826,71 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
@@ -3897,7 +3899,7 @@
         <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3906,53 +3908,53 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" t="s">
         <v>243</v>
       </c>
-      <c r="C1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B2" t="s">
-        <v>244</v>
-      </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3961,44 +3963,44 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Aanpassingen naar aanleiding van lync sessie
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="17310" windowHeight="8115" firstSheet="12" activeTab="19"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="17316" windowHeight="8112"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="9" r:id="rId1"/>
@@ -749,9 +749,6 @@
     <t>FAB</t>
   </si>
   <si>
-    <t>P&amp;O</t>
-  </si>
-  <si>
     <t>Medewerker</t>
   </si>
   <si>
@@ -774,6 +771,9 @@
   </si>
   <si>
     <t>TEXT</t>
+  </si>
+  <si>
+    <t>HR</t>
   </si>
 </sst>
 </file>
@@ -813,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -830,12 +830,10 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="adhoc - Roosters "/>
-      <sheetName val="Bericht"/>
       <sheetName val="Dagverantwoording"/>
       <sheetName val="Modaliteit"/>
       <sheetName val="Personeelsnummer"/>
       <sheetName val="Tijdvak"/>
-      <sheetName val="aan"/>
       <sheetName val="arbeidsmod"/>
       <sheetName val="arbeidsmodaliteitIngangsdatum"/>
       <sheetName val="binnenTijdvak"/>
@@ -844,6 +842,8 @@
       <sheetName val="geqTijdstip"/>
       <sheetName val="gtDatum"/>
       <sheetName val="overlap"/>
+      <sheetName val="Bericht"/>
+      <sheetName val="aan"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -1130,17 +1130,17 @@
       <sheetData sheetId="10"/>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1178,7 +1178,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1250,7 +1250,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1426,19 +1426,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>233</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>232</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -1472,7 +1472,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF('[1]adhoc - Roosters '!A2,TEXT('[1]adhoc - Roosters '!A2,"#"),"")</f>
         <v>7148691</v>
@@ -1487,7 +1487,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
         <v>7151751</v>
@@ -1502,7 +1502,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>20045763</v>
@@ -1514,10 +1514,10 @@
         <v>231</v>
       </c>
       <c r="E5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045773</v>
@@ -1529,10 +1529,10 @@
         <v>231</v>
       </c>
       <c r="E6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20046068</v>
@@ -1544,10 +1544,10 @@
         <v>231</v>
       </c>
       <c r="E7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046310</v>
@@ -1559,10 +1559,10 @@
         <v>231</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046336</v>
@@ -1574,10 +1574,10 @@
         <v>231</v>
       </c>
       <c r="E9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046357</v>
@@ -1589,10 +1589,10 @@
         <v>231</v>
       </c>
       <c r="E10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046480</v>
@@ -1604,10 +1604,10 @@
         <v>231</v>
       </c>
       <c r="E11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046490</v>
@@ -1619,10 +1619,10 @@
         <v>231</v>
       </c>
       <c r="E12" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046544</v>
@@ -1634,10 +1634,10 @@
         <v>231</v>
       </c>
       <c r="E13" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046555</v>
@@ -1649,10 +1649,10 @@
         <v>231</v>
       </c>
       <c r="E14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046575</v>
@@ -1664,10 +1664,10 @@
         <v>231</v>
       </c>
       <c r="E15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046636</v>
@@ -1679,10 +1679,10 @@
         <v>231</v>
       </c>
       <c r="E16" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046659</v>
@@ -1694,10 +1694,10 @@
         <v>231</v>
       </c>
       <c r="E17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046686</v>
@@ -1709,10 +1709,10 @@
         <v>231</v>
       </c>
       <c r="E18" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046693</v>
@@ -1724,10 +1724,10 @@
         <v>231</v>
       </c>
       <c r="E19" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046747</v>
@@ -1739,10 +1739,10 @@
         <v>231</v>
       </c>
       <c r="E20" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046749</v>
@@ -1754,10 +1754,10 @@
         <v>231</v>
       </c>
       <c r="E21" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046812</v>
@@ -1769,10 +1769,10 @@
         <v>231</v>
       </c>
       <c r="E22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046859</v>
@@ -1784,10 +1784,10 @@
         <v>231</v>
       </c>
       <c r="E23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046868</v>
@@ -1799,10 +1799,10 @@
         <v>231</v>
       </c>
       <c r="E24" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046883</v>
@@ -1814,10 +1814,10 @@
         <v>231</v>
       </c>
       <c r="E25" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046949</v>
@@ -1829,10 +1829,10 @@
         <v>231</v>
       </c>
       <c r="E26" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046981</v>
@@ -1844,10 +1844,10 @@
         <v>231</v>
       </c>
       <c r="E27" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046987</v>
@@ -1859,10 +1859,10 @@
         <v>231</v>
       </c>
       <c r="E28" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20047009</v>
@@ -1874,10 +1874,10 @@
         <v>231</v>
       </c>
       <c r="E29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047081</v>
@@ -1889,10 +1889,10 @@
         <v>231</v>
       </c>
       <c r="E30" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047085</v>
@@ -1904,10 +1904,10 @@
         <v>231</v>
       </c>
       <c r="E31" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047108</v>
@@ -1919,10 +1919,10 @@
         <v>231</v>
       </c>
       <c r="E32" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047118</v>
@@ -1934,10 +1934,10 @@
         <v>231</v>
       </c>
       <c r="E33" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047171</v>
@@ -1949,10 +1949,10 @@
         <v>231</v>
       </c>
       <c r="E34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047188</v>
@@ -1964,10 +1964,10 @@
         <v>231</v>
       </c>
       <c r="E35" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047189</v>
@@ -1979,10 +1979,10 @@
         <v>231</v>
       </c>
       <c r="E36" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047277</v>
@@ -1994,10 +1994,10 @@
         <v>231</v>
       </c>
       <c r="E37" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047291</v>
@@ -2009,10 +2009,10 @@
         <v>231</v>
       </c>
       <c r="E38" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047295</v>
@@ -2024,10 +2024,10 @@
         <v>231</v>
       </c>
       <c r="E39" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047296</v>
@@ -2039,10 +2039,10 @@
         <v>231</v>
       </c>
       <c r="E40" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047310</v>
@@ -2054,10 +2054,10 @@
         <v>231</v>
       </c>
       <c r="E41" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047322</v>
@@ -2069,10 +2069,10 @@
         <v>231</v>
       </c>
       <c r="E42" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047330</v>
@@ -2084,10 +2084,10 @@
         <v>231</v>
       </c>
       <c r="E43" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047672</v>
@@ -2099,10 +2099,10 @@
         <v>231</v>
       </c>
       <c r="E44" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047692</v>
@@ -2114,10 +2114,10 @@
         <v>231</v>
       </c>
       <c r="E45" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047712</v>
@@ -2129,10 +2129,10 @@
         <v>231</v>
       </c>
       <c r="E46" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047716</v>
@@ -2144,10 +2144,10 @@
         <v>231</v>
       </c>
       <c r="E47" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047730</v>
@@ -2159,10 +2159,10 @@
         <v>231</v>
       </c>
       <c r="E48" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047748</v>
@@ -2174,10 +2174,10 @@
         <v>231</v>
       </c>
       <c r="E49" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047775</v>
@@ -2189,10 +2189,10 @@
         <v>231</v>
       </c>
       <c r="E50" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047776</v>
@@ -2204,10 +2204,10 @@
         <v>231</v>
       </c>
       <c r="E51" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047805</v>
@@ -2219,10 +2219,10 @@
         <v>231</v>
       </c>
       <c r="E52" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047807</v>
@@ -2234,10 +2234,10 @@
         <v>231</v>
       </c>
       <c r="E53" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047818</v>
@@ -2249,10 +2249,10 @@
         <v>231</v>
       </c>
       <c r="E54" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047832</v>
@@ -2264,10 +2264,10 @@
         <v>231</v>
       </c>
       <c r="E55" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047848</v>
@@ -2279,7 +2279,7 @@
         <v>231</v>
       </c>
       <c r="E56" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2295,12 +2295,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>150</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>151</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>153</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>155</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>156</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>157</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>152</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>164</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>132</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>134</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>136</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>137</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>138</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>140</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>144</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>148</v>
       </c>
@@ -2766,7 +2766,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2795,7 +2795,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2824,7 +2824,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2853,7 +2853,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2882,7 +2882,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2911,7 +2911,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2940,7 +2940,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2969,7 +2969,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3000,7 +3000,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3031,7 +3031,7 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3070,11 +3070,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3103,7 +3103,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3152,7 +3152,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3198,14 +3198,14 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -3213,15 +3213,15 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF('[1]adhoc - Roosters '!A2,TEXT('[1]adhoc - Roosters '!A2,"#"),"")</f>
         <v>7148691</v>
@@ -3230,7 +3230,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
         <v>7151751</v>
@@ -3239,7 +3239,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>20045763</v>
@@ -3248,7 +3248,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045773</v>
@@ -3257,7 +3257,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20046068</v>
@@ -3266,7 +3266,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046310</v>
@@ -3275,7 +3275,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046336</v>
@@ -3284,7 +3284,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046357</v>
@@ -3293,7 +3293,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046480</v>
@@ -3302,7 +3302,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046490</v>
@@ -3311,7 +3311,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046544</v>
@@ -3320,7 +3320,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046555</v>
@@ -3329,7 +3329,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046575</v>
@@ -3338,7 +3338,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046636</v>
@@ -3347,7 +3347,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046659</v>
@@ -3356,7 +3356,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046686</v>
@@ -3365,7 +3365,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046693</v>
@@ -3374,7 +3374,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046747</v>
@@ -3383,7 +3383,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046749</v>
@@ -3392,7 +3392,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046812</v>
@@ -3401,7 +3401,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046859</v>
@@ -3410,7 +3410,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046868</v>
@@ -3419,7 +3419,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046883</v>
@@ -3428,7 +3428,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046949</v>
@@ -3437,7 +3437,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046981</v>
@@ -3446,7 +3446,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046987</v>
@@ -3455,7 +3455,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20047009</v>
@@ -3464,7 +3464,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047081</v>
@@ -3473,7 +3473,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047085</v>
@@ -3482,7 +3482,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047108</v>
@@ -3491,7 +3491,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047118</v>
@@ -3500,7 +3500,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047171</v>
@@ -3509,7 +3509,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047188</v>
@@ -3518,7 +3518,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047189</v>
@@ -3527,7 +3527,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047277</v>
@@ -3536,7 +3536,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047291</v>
@@ -3545,7 +3545,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047295</v>
@@ -3554,7 +3554,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047296</v>
@@ -3563,7 +3563,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047310</v>
@@ -3572,7 +3572,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047322</v>
@@ -3581,7 +3581,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047330</v>
@@ -3590,7 +3590,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047672</v>
@@ -3599,7 +3599,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047692</v>
@@ -3608,7 +3608,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047712</v>
@@ -3617,7 +3617,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047716</v>
@@ -3626,7 +3626,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047730</v>
@@ -3635,7 +3635,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047748</v>
@@ -3644,7 +3644,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047775</v>
@@ -3653,7 +3653,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047776</v>
@@ -3662,7 +3662,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047805</v>
@@ -3671,7 +3671,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047807</v>
@@ -3680,7 +3680,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047818</v>
@@ -3689,7 +3689,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047832</v>
@@ -3698,7 +3698,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047848</v>
@@ -3707,37 +3707,37 @@
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>230</v>
       </c>
@@ -3755,7 +3755,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3776,7 +3776,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,7 +3797,7 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3877,22 +3877,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" t="s">
         <v>99</v>
@@ -3906,10 +3906,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -3934,7 +3934,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Included Arbeidsmodaliteiten.xlsx, and made some modifications in the populations to enable that.
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8472" yWindow="960" windowWidth="12996" windowHeight="8112"/>
+    <workbookView xWindow="7668" yWindow="-12" windowWidth="7680" windowHeight="9864" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="9" r:id="rId1"/>
@@ -15,13 +15,12 @@
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="78">
   <si>
     <t>Loginnaam</t>
   </si>
@@ -260,8 +259,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -307,17 +306,20 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="voor runtime loader"/>
+      <sheetName val="voor debugging"/>
       <sheetName val="adhoc - Roosters "/>
       <sheetName val="Arbeidsmodaliteiten"/>
       <sheetName val="Modaliteit"/>
       <sheetName val="Variables"/>
-      <sheetName val="Mutation"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
         <row r="3">
           <cell r="A3">
             <v>7148691</v>
@@ -589,19 +591,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -639,7 +640,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -673,6 +674,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -707,9 +709,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -882,22 +885,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -914,7 +917,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -931,799 +934,824 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
+        <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
+        <v>7148691</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>7151751</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="str">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045763</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="str">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20045773</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="str">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046068</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="str">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046310</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="str">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046336</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="str">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046357</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="str">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046480</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="str">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046490</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="str">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046544</v>
       </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="str">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046555</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="str">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046575</v>
       </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="str">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046636</v>
       </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="str">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046659</v>
       </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="str">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046686</v>
       </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="str">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046693</v>
       </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="str">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046747</v>
       </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="str">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046749</v>
       </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="str">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046812</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="str">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046859</v>
       </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="str">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046868</v>
       </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="str">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046883</v>
       </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="str">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046949</v>
       </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="str">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046981</v>
       </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="str">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20046987</v>
       </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="str">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047009</v>
       </c>
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="str">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047081</v>
       </c>
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="str">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047085</v>
       </c>
-      <c r="B30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="str">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047108</v>
       </c>
-      <c r="B31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="str">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047118</v>
       </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="str">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047171</v>
       </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="str">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047188</v>
       </c>
-      <c r="B34" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="str">
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047189</v>
       </c>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E36" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="str">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047277</v>
       </c>
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" t="str">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047291</v>
       </c>
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="str">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047295</v>
       </c>
-      <c r="B38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="str">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047296</v>
       </c>
-      <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="str">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047310</v>
       </c>
-      <c r="B40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="str">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047322</v>
       </c>
-      <c r="B41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="str">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047330</v>
       </c>
-      <c r="B42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="str">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047672</v>
       </c>
-      <c r="B43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="str">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047692</v>
       </c>
-      <c r="B44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="str">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047712</v>
       </c>
-      <c r="B45" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="str">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047716</v>
       </c>
-      <c r="B46" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="str">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047730</v>
       </c>
-      <c r="B47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="str">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047748</v>
       </c>
-      <c r="B48" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="str">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047775</v>
       </c>
-      <c r="B49" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="str">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047776</v>
       </c>
-      <c r="B50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" t="s">
-        <v>67</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="str">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047805</v>
       </c>
-      <c r="B51" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="str">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047807</v>
       </c>
-      <c r="B52" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" t="s">
-        <v>67</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" t="str">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047818</v>
       </c>
-      <c r="B53" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" t="s">
-        <v>67</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="B54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="str">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047832</v>
       </c>
-      <c r="B54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" t="s">
-        <v>67</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="B55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="str">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
         <f>IF('[1]adhoc - Roosters '!A56,TEXT('[1]adhoc - Roosters '!A56,"#"),"")</f>
         <v>20047848</v>
       </c>
-      <c r="B55" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" t="s">
-        <v>67</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1732,21 +1760,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1754,7 +1782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1762,7 +1790,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>IF('[1]adhoc - Roosters '!A3,TEXT('[1]adhoc - Roosters '!A3,"#"),"")</f>
         <v>7148691</v>
@@ -1771,7 +1799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>IF('[1]adhoc - Roosters '!A4,TEXT('[1]adhoc - Roosters '!A4,"#"),"")</f>
         <v>7151751</v>
@@ -1780,7 +1808,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>IF('[1]adhoc - Roosters '!A5,TEXT('[1]adhoc - Roosters '!A5,"#"),"")</f>
         <v>20045763</v>
@@ -1789,7 +1817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>IF('[1]adhoc - Roosters '!A6,TEXT('[1]adhoc - Roosters '!A6,"#"),"")</f>
         <v>20045773</v>
@@ -1798,7 +1826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>IF('[1]adhoc - Roosters '!A7,TEXT('[1]adhoc - Roosters '!A7,"#"),"")</f>
         <v>20046068</v>
@@ -1807,7 +1835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>IF('[1]adhoc - Roosters '!A8,TEXT('[1]adhoc - Roosters '!A8,"#"),"")</f>
         <v>20046310</v>
@@ -1816,7 +1844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>IF('[1]adhoc - Roosters '!A9,TEXT('[1]adhoc - Roosters '!A9,"#"),"")</f>
         <v>20046336</v>
@@ -1825,7 +1853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>IF('[1]adhoc - Roosters '!A10,TEXT('[1]adhoc - Roosters '!A10,"#"),"")</f>
         <v>20046357</v>
@@ -1834,7 +1862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>IF('[1]adhoc - Roosters '!A11,TEXT('[1]adhoc - Roosters '!A11,"#"),"")</f>
         <v>20046480</v>
@@ -1843,7 +1871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>IF('[1]adhoc - Roosters '!A12,TEXT('[1]adhoc - Roosters '!A12,"#"),"")</f>
         <v>20046490</v>
@@ -1852,7 +1880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF('[1]adhoc - Roosters '!A13,TEXT('[1]adhoc - Roosters '!A13,"#"),"")</f>
         <v>20046544</v>
@@ -1861,7 +1889,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>IF('[1]adhoc - Roosters '!A14,TEXT('[1]adhoc - Roosters '!A14,"#"),"")</f>
         <v>20046555</v>
@@ -1870,7 +1898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>IF('[1]adhoc - Roosters '!A15,TEXT('[1]adhoc - Roosters '!A15,"#"),"")</f>
         <v>20046575</v>
@@ -1879,7 +1907,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>IF('[1]adhoc - Roosters '!A16,TEXT('[1]adhoc - Roosters '!A16,"#"),"")</f>
         <v>20046636</v>
@@ -1888,7 +1916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>IF('[1]adhoc - Roosters '!A17,TEXT('[1]adhoc - Roosters '!A17,"#"),"")</f>
         <v>20046659</v>
@@ -1897,7 +1925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>IF('[1]adhoc - Roosters '!A18,TEXT('[1]adhoc - Roosters '!A18,"#"),"")</f>
         <v>20046686</v>
@@ -1906,7 +1934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>IF('[1]adhoc - Roosters '!A19,TEXT('[1]adhoc - Roosters '!A19,"#"),"")</f>
         <v>20046693</v>
@@ -1915,7 +1943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>IF('[1]adhoc - Roosters '!A20,TEXT('[1]adhoc - Roosters '!A20,"#"),"")</f>
         <v>20046747</v>
@@ -1924,7 +1952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>IF('[1]adhoc - Roosters '!A21,TEXT('[1]adhoc - Roosters '!A21,"#"),"")</f>
         <v>20046749</v>
@@ -1933,7 +1961,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>IF('[1]adhoc - Roosters '!A22,TEXT('[1]adhoc - Roosters '!A22,"#"),"")</f>
         <v>20046812</v>
@@ -1942,7 +1970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>IF('[1]adhoc - Roosters '!A23,TEXT('[1]adhoc - Roosters '!A23,"#"),"")</f>
         <v>20046859</v>
@@ -1951,7 +1979,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>IF('[1]adhoc - Roosters '!A24,TEXT('[1]adhoc - Roosters '!A24,"#"),"")</f>
         <v>20046868</v>
@@ -1960,7 +1988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>IF('[1]adhoc - Roosters '!A25,TEXT('[1]adhoc - Roosters '!A25,"#"),"")</f>
         <v>20046883</v>
@@ -1969,7 +1997,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>IF('[1]adhoc - Roosters '!A26,TEXT('[1]adhoc - Roosters '!A26,"#"),"")</f>
         <v>20046949</v>
@@ -1978,7 +2006,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>IF('[1]adhoc - Roosters '!A27,TEXT('[1]adhoc - Roosters '!A27,"#"),"")</f>
         <v>20046981</v>
@@ -1987,7 +2015,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>IF('[1]adhoc - Roosters '!A28,TEXT('[1]adhoc - Roosters '!A28,"#"),"")</f>
         <v>20046987</v>
@@ -1996,7 +2024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>IF('[1]adhoc - Roosters '!A29,TEXT('[1]adhoc - Roosters '!A29,"#"),"")</f>
         <v>20047009</v>
@@ -2005,7 +2033,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>IF('[1]adhoc - Roosters '!A30,TEXT('[1]adhoc - Roosters '!A30,"#"),"")</f>
         <v>20047081</v>
@@ -2014,7 +2042,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>IF('[1]adhoc - Roosters '!A31,TEXT('[1]adhoc - Roosters '!A31,"#"),"")</f>
         <v>20047085</v>
@@ -2023,7 +2051,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>IF('[1]adhoc - Roosters '!A32,TEXT('[1]adhoc - Roosters '!A32,"#"),"")</f>
         <v>20047108</v>
@@ -2032,7 +2060,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>IF('[1]adhoc - Roosters '!A33,TEXT('[1]adhoc - Roosters '!A33,"#"),"")</f>
         <v>20047118</v>
@@ -2041,7 +2069,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>IF('[1]adhoc - Roosters '!A34,TEXT('[1]adhoc - Roosters '!A34,"#"),"")</f>
         <v>20047171</v>
@@ -2050,7 +2078,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>IF('[1]adhoc - Roosters '!A35,TEXT('[1]adhoc - Roosters '!A35,"#"),"")</f>
         <v>20047188</v>
@@ -2059,7 +2087,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>IF('[1]adhoc - Roosters '!A36,TEXT('[1]adhoc - Roosters '!A36,"#"),"")</f>
         <v>20047189</v>
@@ -2068,7 +2096,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>IF('[1]adhoc - Roosters '!A37,TEXT('[1]adhoc - Roosters '!A37,"#"),"")</f>
         <v>20047277</v>
@@ -2077,7 +2105,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>IF('[1]adhoc - Roosters '!A38,TEXT('[1]adhoc - Roosters '!A38,"#"),"")</f>
         <v>20047291</v>
@@ -2086,7 +2114,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>IF('[1]adhoc - Roosters '!A39,TEXT('[1]adhoc - Roosters '!A39,"#"),"")</f>
         <v>20047295</v>
@@ -2095,7 +2123,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>IF('[1]adhoc - Roosters '!A40,TEXT('[1]adhoc - Roosters '!A40,"#"),"")</f>
         <v>20047296</v>
@@ -2104,7 +2132,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>IF('[1]adhoc - Roosters '!A41,TEXT('[1]adhoc - Roosters '!A41,"#"),"")</f>
         <v>20047310</v>
@@ -2113,7 +2141,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>IF('[1]adhoc - Roosters '!A42,TEXT('[1]adhoc - Roosters '!A42,"#"),"")</f>
         <v>20047322</v>
@@ -2122,7 +2150,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>IF('[1]adhoc - Roosters '!A43,TEXT('[1]adhoc - Roosters '!A43,"#"),"")</f>
         <v>20047330</v>
@@ -2131,7 +2159,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f>IF('[1]adhoc - Roosters '!A44,TEXT('[1]adhoc - Roosters '!A44,"#"),"")</f>
         <v>20047672</v>
@@ -2140,7 +2168,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>IF('[1]adhoc - Roosters '!A45,TEXT('[1]adhoc - Roosters '!A45,"#"),"")</f>
         <v>20047692</v>
@@ -2149,7 +2177,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f>IF('[1]adhoc - Roosters '!A46,TEXT('[1]adhoc - Roosters '!A46,"#"),"")</f>
         <v>20047712</v>
@@ -2158,7 +2186,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f>IF('[1]adhoc - Roosters '!A47,TEXT('[1]adhoc - Roosters '!A47,"#"),"")</f>
         <v>20047716</v>
@@ -2167,7 +2195,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f>IF('[1]adhoc - Roosters '!A48,TEXT('[1]adhoc - Roosters '!A48,"#"),"")</f>
         <v>20047730</v>
@@ -2176,7 +2204,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f>IF('[1]adhoc - Roosters '!A49,TEXT('[1]adhoc - Roosters '!A49,"#"),"")</f>
         <v>20047748</v>
@@ -2185,7 +2213,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f>IF('[1]adhoc - Roosters '!A50,TEXT('[1]adhoc - Roosters '!A50,"#"),"")</f>
         <v>20047775</v>
@@ -2194,7 +2222,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>IF('[1]adhoc - Roosters '!A51,TEXT('[1]adhoc - Roosters '!A51,"#"),"")</f>
         <v>20047776</v>
@@ -2203,7 +2231,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>IF('[1]adhoc - Roosters '!A52,TEXT('[1]adhoc - Roosters '!A52,"#"),"")</f>
         <v>20047805</v>
@@ -2212,7 +2240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="str">
         <f>IF('[1]adhoc - Roosters '!A53,TEXT('[1]adhoc - Roosters '!A53,"#"),"")</f>
         <v>20047807</v>
@@ -2221,7 +2249,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="str">
         <f>IF('[1]adhoc - Roosters '!A54,TEXT('[1]adhoc - Roosters '!A54,"#"),"")</f>
         <v>20047818</v>
@@ -2230,7 +2258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="str">
         <f>IF('[1]adhoc - Roosters '!A55,TEXT('[1]adhoc - Roosters '!A55,"#"),"")</f>
         <v>20047832</v>
@@ -2239,17 +2267,29 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
+        <f>IF('[1]adhoc - Roosters '!A56,TEXT('[1]adhoc - Roosters '!A56,"#"),"")</f>
+        <v>20047848</v>
+      </c>
       <c r="B56" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="str">
+        <f>IF('[1]adhoc - Roosters '!A57,TEXT('[1]adhoc - Roosters '!A57,"#"),"")</f>
+        <v/>
+      </c>
       <c r="B57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="str">
+        <f>IF('[1]adhoc - Roosters '!A58,TEXT('[1]adhoc - Roosters '!A58,"#"),"")</f>
+        <v/>
+      </c>
       <c r="B58" t="s">
         <v>66</v>
       </c>
@@ -2260,16 +2300,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2280,7 +2320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2297,12 +2337,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
vertaalbaar maken t.b.v. gegevensmodel NVWA
</commit_message>
<xml_diff>
--- a/NVWA DTV/DTV_populaties.xlsx
+++ b/NVWA DTV/DTV_populaties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="12996" windowHeight="8112" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="12996" windowHeight="8112" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="9" r:id="rId1"/>
@@ -16,25 +16,26 @@
     <sheet name="Tijdvak" sheetId="12" r:id="rId7"/>
     <sheet name="ToelageResultaat" sheetId="13" r:id="rId8"/>
     <sheet name="Urentegoed" sheetId="14" r:id="rId9"/>
-    <sheet name="Variable" sheetId="15" r:id="rId10"/>
-    <sheet name="date" sheetId="20" r:id="rId11"/>
-    <sheet name="geldigOp" sheetId="21" r:id="rId12"/>
-    <sheet name="geqDatum" sheetId="22" r:id="rId13"/>
-    <sheet name="geqTijdstip" sheetId="23" r:id="rId14"/>
-    <sheet name="gtDatum" sheetId="24" r:id="rId15"/>
-    <sheet name="overlap1" sheetId="25" r:id="rId16"/>
-    <sheet name="overlap2" sheetId="26" r:id="rId17"/>
-    <sheet name="Blad1" sheetId="27" r:id="rId18"/>
+    <sheet name="StamItem" sheetId="28" r:id="rId10"/>
+    <sheet name="Variable" sheetId="15" r:id="rId11"/>
+    <sheet name="date" sheetId="20" r:id="rId12"/>
+    <sheet name="geldigOp" sheetId="21" r:id="rId13"/>
+    <sheet name="geqDatum" sheetId="22" r:id="rId14"/>
+    <sheet name="geqTijdstip" sheetId="23" r:id="rId15"/>
+    <sheet name="gtDatum" sheetId="24" r:id="rId16"/>
+    <sheet name="overlap1" sheetId="25" r:id="rId17"/>
+    <sheet name="overlap2" sheetId="26" r:id="rId18"/>
+    <sheet name="Blad1" sheetId="27" r:id="rId19"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
   </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="242">
   <si>
     <t>ARAR Artikel 37a + 37b</t>
   </si>
@@ -754,6 +755,12 @@
   </si>
   <si>
     <t>TEXT</t>
+  </si>
+  <si>
+    <t>StamItem</t>
+  </si>
+  <si>
+    <t>[StamItem]</t>
   </si>
 </sst>
 </file>
@@ -2242,20 +2249,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>241</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -2267,18 +2271,12 @@
         <v>160</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>240</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -2287,16 +2285,10 @@
         <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -2306,11 +2298,11 @@
       <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>144</v>
       </c>
@@ -2320,11 +2312,11 @@
       <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -2334,11 +2326,11 @@
       <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>147</v>
       </c>
@@ -2348,11 +2340,11 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -2362,11 +2354,11 @@
       <c r="D7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -2376,11 +2368,11 @@
       <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -2390,11 +2382,11 @@
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>151</v>
       </c>
@@ -2404,11 +2396,11 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>152</v>
       </c>
@@ -2418,293 +2410,293 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>124</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>135</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>146</v>
       </c>
       <c r="D14" t="s">
         <v>63</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>153</v>
       </c>
       <c r="D15" t="s">
         <v>65</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>154</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>155</v>
       </c>
       <c r="D17" t="s">
         <v>64</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>156</v>
       </c>
       <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>157</v>
       </c>
       <c r="D19" t="s">
         <v>68</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>158</v>
       </c>
       <c r="D20" t="s">
         <v>97</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>125</v>
       </c>
       <c r="D21" t="s">
         <v>107</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>126</v>
       </c>
       <c r="D22" t="s">
         <v>108</v>
       </c>
-      <c r="F22" t="s">
+      <c r="E22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>127</v>
       </c>
       <c r="D23" t="s">
         <v>109</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>128</v>
       </c>
       <c r="D24" t="s">
         <v>110</v>
       </c>
-      <c r="F24" t="s">
+      <c r="E24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>129</v>
       </c>
       <c r="D25" t="s">
         <v>111</v>
       </c>
-      <c r="F25" t="s">
+      <c r="E25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>130</v>
       </c>
       <c r="D26" t="s">
         <v>112</v>
       </c>
-      <c r="F26" t="s">
+      <c r="E26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>131</v>
       </c>
       <c r="D27" t="s">
         <v>113</v>
       </c>
-      <c r="F27" t="s">
+      <c r="E27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>132</v>
       </c>
       <c r="D28" t="s">
         <v>114</v>
       </c>
-      <c r="F28" t="s">
+      <c r="E28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>133</v>
       </c>
       <c r="D29" t="s">
         <v>98</v>
       </c>
-      <c r="F29" t="s">
+      <c r="E29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>134</v>
       </c>
       <c r="D30" t="s">
         <v>99</v>
       </c>
-      <c r="F30" t="s">
+      <c r="E30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>136</v>
       </c>
       <c r="D31" t="s">
         <v>100</v>
       </c>
-      <c r="F31" t="s">
+      <c r="E31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>137</v>
       </c>
       <c r="D32" t="s">
         <v>101</v>
       </c>
-      <c r="F32" t="s">
+      <c r="E32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>138</v>
       </c>
       <c r="D33" t="s">
         <v>102</v>
       </c>
-      <c r="F33" t="s">
+      <c r="E33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>139</v>
       </c>
       <c r="D34" t="s">
         <v>103</v>
       </c>
-      <c r="F34" t="s">
+      <c r="E34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>140</v>
       </c>
       <c r="D35" t="s">
         <v>104</v>
       </c>
-      <c r="F35" t="s">
+      <c r="E35" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>141</v>
       </c>
       <c r="D36" t="s">
         <v>105</v>
       </c>
-      <c r="F36" t="s">
+      <c r="E36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>142</v>
       </c>
       <c r="D37" t="s">
         <v>106</v>
       </c>
-      <c r="F37" t="s">
+      <c r="E37" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2715,26 +2707,209 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2752,15 +2927,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -2781,15 +2956,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -2810,18 +2985,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2839,18 +3014,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2859,6 +3034,35 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2889,7 +3093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2920,11 +3124,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>

</xml_diff>